<commit_message>
From v1.0.1 to v1.0.2
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
+++ b/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
@@ -92,6 +92,120 @@
     <t>Actual Result</t>
   </si>
   <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de viagem nacional - fora do estado (interestadual).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: viagem nacional - fora do estado (interestadual).</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o estado.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: estado.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe a(s) cidade(s).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: cidade(s).</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de deslocamento.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: tipo de deslocamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de hospedagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: hospedagem.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de periodo de afastamento.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: periodo de afastamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa as datas de afastamento, apos o ultimo dia de viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: pernoite.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Detalha a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe os beneficiarios selecionados.</t>
+  </si>
+  <si>
+    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Clica em confirmar.</t>
+  </si>
+  <si>
+    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado.</t>
+  </si>
+  <si>
+    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>O sistema salva os dados</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa as datas de afastamento ALTERNADAS, antes do ultimo dia de viagem.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Clica em limpar campos.</t>
+  </si>
+  <si>
+    <t>SYSTEM Apaga todas as seleções do usuário.</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
     <t>Chefe/Beneficiário Seleciona o tipo de viagem nacional - dentro do estado (intermunicipal).</t>
   </si>
   <si>
@@ -104,136 +218,22 @@
     <t>SYSTEM O sistema seleciona o estado como PB, automaticamente.</t>
   </si>
   <si>
-    <t>Chefe/Beneficiário Escolhe a(s) cidade(s).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: cidade(s).</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de deslocamento.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: tipo de deslocamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de hospedagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: hospedagem.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de periodo de afastamento.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: periodo de afastamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa as datas de afastamento, apos o ultimo dia de viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: pernoite.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Detalha a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe os beneficiarios selecionados.</t>
-  </si>
-  <si>
-    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Clica em confirmar.</t>
-  </si>
-  <si>
-    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado.</t>
-  </si>
-  <si>
-    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>O sistema salva os dados</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa as datas de afastamento ALTERNADAS, antes do ultimo dia de viagem.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Clica em limpar campos.</t>
-  </si>
-  <si>
-    <t>SYSTEM Apaga todas as seleções do usuário.</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de viagem nacional - fora do estado (interestadual).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: viagem nacional - fora do estado (interestadual).</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o estado.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: estado.</t>
-  </si>
-  <si>
     <t>Chefe/Beneficiário Informa as datas de afastamento, antes do ultimo dia de viagem.</t>
   </si>
   <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG203 - Campos obrigatórios, MSG214 - Campos obrigatórios da solicitação de diárias (não informados).</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
     <t>SYSTEM Exibe a mensagem de erro MSG202 - RGP Core indisponível.</t>
-  </si>
-  <si>
-    <t>TC4</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
-  </si>
-  <si>
-    <t>TC5</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG203 - Campos obrigatórios, MSG214 - Campos obrigatórios da solicitação de diárias (não informados).</t>
   </si>
   <si>
     <t>TC6</t>
@@ -1526,129 +1526,129 @@
         <v>2</v>
       </c>
       <c r="D60" t="s" s="7">
+        <v>48</v>
+      </c>
+      <c r="E60" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F60" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n" s="10">
+        <v>13.0</v>
+      </c>
+      <c r="B61" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="C61" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s" s="7">
         <v>69</v>
       </c>
-      <c r="E60" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F60" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61"/>
+      <c r="E61" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F61" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="62"/>
-    <row r="63">
-      <c r="A63" t="s" s="4">
+    <row r="63"/>
+    <row r="64">
+      <c r="A64" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B63" t="s" s="4">
+      <c r="B64" t="s" s="4">
         <v>70</v>
       </c>
-      <c r="C63" t="s" s="4">
+      <c r="C64" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D63" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E63" t="s" s="4">
+      <c r="D64" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F63" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s" s="9">
+      <c r="F64" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E64" t="s" s="9">
+      <c r="B65" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F64" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s" s="8">
+      <c r="F65" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B65" t="s" s="8">
+      <c r="B66" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F65" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s" s="5">
+      <c r="C66" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E66" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F66" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B66" t="s" s="5">
+      <c r="B67" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C66" t="s" s="5">
+      <c r="C67" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D66" t="s" s="5">
+      <c r="D67" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E66" t="s" s="5">
+      <c r="E67" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F66" t="s" s="5">
+      <c r="F67" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B67" t="s" s="7">
-        <v>56</v>
-      </c>
-      <c r="C67" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D67" t="s" s="7">
-        <v>57</v>
-      </c>
-      <c r="E67" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F67" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n" s="10">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B68" t="s" s="7">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="C68" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D68" t="s" s="7">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E68" t="s" s="6">
         <v>2</v>
@@ -1659,16 +1659,16 @@
     </row>
     <row r="69">
       <c r="A69" t="n" s="10">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B69" t="s" s="7">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="C69" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D69" t="s" s="7">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="E69" t="s" s="6">
         <v>2</v>
@@ -1679,16 +1679,16 @@
     </row>
     <row r="70">
       <c r="A70" t="n" s="10">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B70" t="s" s="7">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C70" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D70" t="s" s="7">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E70" t="s" s="6">
         <v>2</v>
@@ -1699,16 +1699,16 @@
     </row>
     <row r="71">
       <c r="A71" t="n" s="10">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B71" t="s" s="7">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C71" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D71" t="s" s="7">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E71" t="s" s="6">
         <v>2</v>
@@ -1719,16 +1719,16 @@
     </row>
     <row r="72">
       <c r="A72" t="n" s="10">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B72" t="s" s="7">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C72" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D72" t="s" s="7">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E72" t="s" s="6">
         <v>2</v>
@@ -1739,16 +1739,16 @@
     </row>
     <row r="73">
       <c r="A73" t="n" s="10">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B73" t="s" s="7">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C73" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D73" t="s" s="7">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E73" t="s" s="6">
         <v>2</v>
@@ -1759,16 +1759,16 @@
     </row>
     <row r="74">
       <c r="A74" t="n" s="10">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B74" t="s" s="7">
-        <v>42</v>
+        <v>68</v>
       </c>
       <c r="C74" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D74" t="s" s="7">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E74" t="s" s="6">
         <v>2</v>
@@ -1779,16 +1779,16 @@
     </row>
     <row r="75">
       <c r="A75" t="n" s="10">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B75" t="s" s="7">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C75" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D75" t="s" s="7">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E75" t="s" s="6">
         <v>2</v>
@@ -1799,16 +1799,16 @@
     </row>
     <row r="76">
       <c r="A76" t="n" s="10">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="B76" t="s" s="7">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C76" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D76" t="s" s="7">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E76" t="s" s="6">
         <v>2</v>
@@ -1819,16 +1819,16 @@
     </row>
     <row r="77">
       <c r="A77" t="n" s="10">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="B77" t="s" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C77" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D77" t="s" s="7">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E77" t="s" s="6">
         <v>2</v>
@@ -1839,158 +1839,158 @@
     </row>
     <row r="78">
       <c r="A78" t="n" s="10">
+        <v>11.0</v>
+      </c>
+      <c r="B78" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C78" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s" s="7">
+        <v>47</v>
+      </c>
+      <c r="E78" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F78" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n" s="10">
         <v>12.0</v>
       </c>
-      <c r="B78" t="s" s="7">
+      <c r="B79" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C79" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s" s="7">
+        <v>48</v>
+      </c>
+      <c r="E79" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F79" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n" s="10">
+        <v>13.0</v>
+      </c>
+      <c r="B80" t="s" s="7">
         <v>49</v>
       </c>
-      <c r="C78" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D78" t="s" s="7">
+      <c r="C80" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D80" t="s" s="7">
         <v>71</v>
       </c>
-      <c r="E78" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F78" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79"/>
-    <row r="80"/>
-    <row r="81">
-      <c r="A81" t="s" s="4">
+      <c r="E80" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F80" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83">
+      <c r="A83" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B81" t="s" s="4">
+      <c r="B83" t="s" s="4">
         <v>72</v>
       </c>
-      <c r="C81" t="s" s="4">
+      <c r="C83" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D81" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E81" t="s" s="4">
+      <c r="D83" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E83" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F81" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s" s="9">
+      <c r="F83" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B82" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C82" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D82" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E82" t="s" s="9">
+      <c r="B84" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C84" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E84" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F82" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s" s="8">
+      <c r="F84" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B83" t="s" s="8">
+      <c r="B85" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C83" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D83" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E83" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F83" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s" s="5">
+      <c r="C85" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D85" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E85" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F85" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B84" t="s" s="5">
+      <c r="B86" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C84" t="s" s="5">
+      <c r="C86" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D84" t="s" s="5">
+      <c r="D86" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E84" t="s" s="5">
+      <c r="E86" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F84" t="s" s="5">
+      <c r="F86" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B85" t="s" s="7">
-        <v>64</v>
-      </c>
-      <c r="C85" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D85" t="s" s="7">
-        <v>65</v>
-      </c>
-      <c r="E85" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F85" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="n" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="B86" t="s" s="7">
-        <v>66</v>
-      </c>
-      <c r="C86" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D86" t="s" s="7">
-        <v>67</v>
-      </c>
-      <c r="E86" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F86" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n" s="10">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B87" t="s" s="7">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C87" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D87" t="s" s="7">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="E87" t="s" s="6">
         <v>2</v>
@@ -2001,16 +2001,16 @@
     </row>
     <row r="88">
       <c r="A88" t="n" s="10">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="B88" t="s" s="7">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="C88" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D88" t="s" s="7">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="E88" t="s" s="6">
         <v>2</v>
@@ -2021,16 +2021,16 @@
     </row>
     <row r="89">
       <c r="A89" t="n" s="10">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="B89" t="s" s="7">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C89" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D89" t="s" s="7">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E89" t="s" s="6">
         <v>2</v>
@@ -2041,16 +2041,16 @@
     </row>
     <row r="90">
       <c r="A90" t="n" s="10">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="B90" t="s" s="7">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C90" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D90" t="s" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E90" t="s" s="6">
         <v>2</v>
@@ -2061,16 +2061,16 @@
     </row>
     <row r="91">
       <c r="A91" t="n" s="10">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="B91" t="s" s="7">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C91" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D91" t="s" s="7">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E91" t="s" s="6">
         <v>2</v>
@@ -2081,16 +2081,16 @@
     </row>
     <row r="92">
       <c r="A92" t="n" s="10">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="B92" t="s" s="7">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C92" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D92" t="s" s="7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E92" t="s" s="6">
         <v>2</v>
@@ -2101,16 +2101,16 @@
     </row>
     <row r="93">
       <c r="A93" t="n" s="10">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
       <c r="B93" t="s" s="7">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C93" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D93" t="s" s="7">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E93" t="s" s="6">
         <v>2</v>
@@ -2121,16 +2121,16 @@
     </row>
     <row r="94">
       <c r="A94" t="n" s="10">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="B94" t="s" s="7">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C94" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D94" t="s" s="7">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E94" t="s" s="6">
         <v>2</v>
@@ -2141,16 +2141,16 @@
     </row>
     <row r="95">
       <c r="A95" t="n" s="10">
-        <v>11.0</v>
+        <v>9.0</v>
       </c>
       <c r="B95" t="s" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C95" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D95" t="s" s="7">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E95" t="s" s="6">
         <v>2</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="96">
       <c r="A96" t="n" s="10">
-        <v>12.0</v>
+        <v>10.0</v>
       </c>
       <c r="B96" t="s" s="7">
         <v>46</v>
@@ -2170,7 +2170,7 @@
         <v>2</v>
       </c>
       <c r="D96" t="s" s="7">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E96" t="s" s="6">
         <v>2</v>
@@ -2181,10 +2181,10 @@
     </row>
     <row r="97">
       <c r="A97" t="n" s="10">
-        <v>13.0</v>
+        <v>11.0</v>
       </c>
       <c r="B97" t="s" s="7">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C97" t="s" s="6">
         <v>2</v>
@@ -2286,13 +2286,13 @@
         <v>1.0</v>
       </c>
       <c r="B104" t="s" s="7">
-        <v>64</v>
+        <v>26</v>
       </c>
       <c r="C104" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D104" t="s" s="7">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="E104" t="s" s="6">
         <v>2</v>
@@ -2306,7 +2306,7 @@
         <v>2.0</v>
       </c>
       <c r="B105" t="s" s="7">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="C105" t="s" s="6">
         <v>2</v>
@@ -2331,10 +2331,10 @@
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="B85:F85"/>
     <mergeCell ref="B101:D101"/>
     <mergeCell ref="B102:F102"/>
   </mergeCells>

</xml_diff>

<commit_message>
From v1.0.2 to v1.0.3
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
+++ b/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="75">
   <si>
     <t xml:space="preserve">System: </t>
   </si>
@@ -92,6 +92,120 @@
     <t>Actual Result</t>
   </si>
   <si>
+    <t>Chefe/Beneficiário Seleciona o tipo de viagem nacional - dentro do estado (intermunicipal).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: viagem nacional - dentro do estado (intermunicipal)</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário NÃO Escolhe o estado.</t>
+  </si>
+  <si>
+    <t>SYSTEM O sistema seleciona o estado como PB, automaticamente.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe a(s) cidade(s).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: cidade(s).</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de deslocamento.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: tipo de deslocamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de hospedagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: hospedagem.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de periodo de afastamento.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: periodo de afastamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa as datas de afastamento, antes do ultimo dia de viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: pernoite.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Detalha a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe os beneficiarios selecionados.</t>
+  </si>
+  <si>
+    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Clica em confirmar.</t>
+  </si>
+  <si>
+    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado.</t>
+  </si>
+  <si>
+    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>O sistema salva os dados</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa as datas de afastamento, apos o ultimo dia de viagem.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Clica em limpar campos.</t>
+  </si>
+  <si>
+    <t>SYSTEM Apaga todas as seleções do usuário.</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
     <t>Chefe/Beneficiário Escolhe o tipo de viagem nacional - fora do estado (interestadual).</t>
   </si>
   <si>
@@ -104,142 +218,25 @@
     <t>SYSTEM Exibe a opcao escolhida: estado.</t>
   </si>
   <si>
-    <t>Chefe/Beneficiário Escolhe a(s) cidade(s).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: cidade(s).</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de deslocamento.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: tipo de deslocamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de hospedagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: hospedagem.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de periodo de afastamento.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: periodo de afastamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa as datas de afastamento, apos o ultimo dia de viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: pernoite.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Detalha a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe os beneficiarios selecionados.</t>
-  </si>
-  <si>
-    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Clica em confirmar.</t>
-  </si>
-  <si>
-    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado.</t>
-  </si>
-  <si>
-    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>O sistema salva os dados</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa as datas de afastamento ALTERNADAS, antes do ultimo dia de viagem.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Clica em limpar campos.</t>
-  </si>
-  <si>
-    <t>SYSTEM Apaga todas as seleções do usuário.</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o tipo de viagem nacional - dentro do estado (intermunicipal).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: viagem nacional - dentro do estado (intermunicipal)</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário NÃO Escolhe o estado.</t>
-  </si>
-  <si>
-    <t>SYSTEM O sistema seleciona o estado como PB, automaticamente.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa as datas de afastamento, antes do ultimo dia de viagem.</t>
-  </si>
-  <si>
     <t>SYSTEM Exibe a mensagem de erro MSG203 - Campos obrigatórios, MSG214 - Campos obrigatórios da solicitação de diárias (não informados).</t>
   </si>
   <si>
     <t>TC4</t>
   </si>
   <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG201 - DNE indisponível.</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
     <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
   </si>
   <si>
-    <t>TC5</t>
+    <t>TC6</t>
   </si>
   <si>
     <t>SYSTEM Exibe a mensagem de erro MSG202 - RGP Core indisponível.</t>
-  </si>
-  <si>
-    <t>TC6</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG201 - DNE indisponível.</t>
   </si>
 </sst>
 </file>
@@ -1420,7 +1417,7 @@
         <v>7.0</v>
       </c>
       <c r="B55" t="s" s="7">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C55" t="s" s="6">
         <v>2</v>
@@ -1546,7 +1543,7 @@
         <v>2</v>
       </c>
       <c r="D61" t="s" s="7">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E61" t="s" s="6">
         <v>2</v>
@@ -1562,7 +1559,7 @@
         <v>12</v>
       </c>
       <c r="B64" t="s" s="4">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C64" t="s" s="4">
         <v>14</v>
@@ -1668,7 +1665,7 @@
         <v>2</v>
       </c>
       <c r="D69" t="s" s="7">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="E69" t="s" s="6">
         <v>2</v>
@@ -1677,138 +1674,100 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="n" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="B70" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="C70" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D70" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="E70" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F70" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="n" s="10">
-        <v>4.0</v>
-      </c>
-      <c r="B71" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="C71" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D71" t="s" s="7">
-        <v>33</v>
-      </c>
-      <c r="E71" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F71" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="70"/>
+    <row r="71"/>
     <row r="72">
-      <c r="A72" t="n" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="B72" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="C72" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D72" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="E72" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F72" t="s" s="6">
+      <c r="A72" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B72" t="s" s="4">
+        <v>71</v>
+      </c>
+      <c r="C72" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D72" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E72" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F72" t="s" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="n" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="B73" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="C73" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D73" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="E73" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F73" t="s" s="6">
+      <c r="A73" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B73" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C73" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D73" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E73" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F73" t="s" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="n" s="10">
-        <v>7.0</v>
-      </c>
-      <c r="B74" t="s" s="7">
-        <v>68</v>
-      </c>
-      <c r="C74" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D74" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="E74" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F74" t="s" s="6">
+      <c r="A74" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B74" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C74" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E74" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F74" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="n" s="10">
-        <v>8.0</v>
-      </c>
-      <c r="B75" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="C75" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D75" t="s" s="7">
-        <v>41</v>
-      </c>
-      <c r="E75" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F75" t="s" s="6">
-        <v>2</v>
+      <c r="A75" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B75" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C75" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D75" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E75" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F75" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n" s="10">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
       <c r="B76" t="s" s="7">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C76" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D76" t="s" s="7">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E76" t="s" s="6">
         <v>2</v>
@@ -1819,16 +1778,16 @@
     </row>
     <row r="77">
       <c r="A77" t="n" s="10">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
       <c r="B77" t="s" s="7">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C77" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D77" t="s" s="7">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="E77" t="s" s="6">
         <v>2</v>
@@ -1839,16 +1798,16 @@
     </row>
     <row r="78">
       <c r="A78" t="n" s="10">
-        <v>11.0</v>
+        <v>3.0</v>
       </c>
       <c r="B78" t="s" s="7">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="C78" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D78" t="s" s="7">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="E78" t="s" s="6">
         <v>2</v>
@@ -1859,16 +1818,16 @@
     </row>
     <row r="79">
       <c r="A79" t="n" s="10">
-        <v>12.0</v>
+        <v>4.0</v>
       </c>
       <c r="B79" t="s" s="7">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C79" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D79" t="s" s="7">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="E79" t="s" s="6">
         <v>2</v>
@@ -1879,16 +1838,16 @@
     </row>
     <row r="80">
       <c r="A80" t="n" s="10">
-        <v>13.0</v>
+        <v>5.0</v>
       </c>
       <c r="B80" t="s" s="7">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C80" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D80" t="s" s="7">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="E80" t="s" s="6">
         <v>2</v>
@@ -1897,100 +1856,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="81"/>
-    <row r="82"/>
+    <row r="81">
+      <c r="A81" t="n" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="B81" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="C81" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="E81" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F81" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n" s="10">
+        <v>7.0</v>
+      </c>
+      <c r="B82" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="C82" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="E82" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F82" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="83">
-      <c r="A83" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B83" t="s" s="4">
-        <v>72</v>
-      </c>
-      <c r="C83" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D83" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E83" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F83" t="s" s="4">
+      <c r="A83" t="n" s="10">
+        <v>8.0</v>
+      </c>
+      <c r="B83" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="C83" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D83" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="E83" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F83" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B84" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C84" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D84" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E84" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F84" t="s" s="9">
+      <c r="A84" t="n" s="10">
+        <v>9.0</v>
+      </c>
+      <c r="B84" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="C84" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="E84" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F84" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B85" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C85" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D85" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E85" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F85" t="s" s="8">
+      <c r="A85" t="n" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="B85" t="s" s="7">
+        <v>44</v>
+      </c>
+      <c r="C85" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D85" t="s" s="7">
+        <v>45</v>
+      </c>
+      <c r="E85" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F85" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B86" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C86" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D86" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E86" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F86" t="s" s="5">
-        <v>25</v>
+      <c r="A86" t="n" s="10">
+        <v>11.0</v>
+      </c>
+      <c r="B86" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C86" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D86" t="s" s="7">
+        <v>47</v>
+      </c>
+      <c r="E86" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F86" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n" s="10">
-        <v>1.0</v>
+        <v>12.0</v>
       </c>
       <c r="B87" t="s" s="7">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C87" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D87" t="s" s="7">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E87" t="s" s="6">
         <v>2</v>
@@ -2001,16 +1998,16 @@
     </row>
     <row r="88">
       <c r="A88" t="n" s="10">
-        <v>2.0</v>
+        <v>13.0</v>
       </c>
       <c r="B88" t="s" s="7">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C88" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D88" t="s" s="7">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="E88" t="s" s="6">
         <v>2</v>
@@ -2019,138 +2016,100 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" t="n" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="B89" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="C89" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D89" t="s" s="7">
-        <v>33</v>
-      </c>
-      <c r="E89" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F89" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="n" s="10">
-        <v>4.0</v>
-      </c>
-      <c r="B90" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="C90" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D90" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="E90" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F90" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="89"/>
+    <row r="90"/>
     <row r="91">
-      <c r="A91" t="n" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="B91" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="C91" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D91" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="E91" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F91" t="s" s="6">
+      <c r="A91" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B91" t="s" s="4">
+        <v>73</v>
+      </c>
+      <c r="C91" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D91" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E91" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F91" t="s" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="n" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="B92" t="s" s="7">
-        <v>68</v>
-      </c>
-      <c r="C92" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D92" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="E92" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F92" t="s" s="6">
+      <c r="A92" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B92" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C92" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D92" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E92" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F92" t="s" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="n" s="10">
-        <v>7.0</v>
-      </c>
-      <c r="B93" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="C93" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D93" t="s" s="7">
-        <v>41</v>
-      </c>
-      <c r="E93" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F93" t="s" s="6">
+      <c r="A93" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B93" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C93" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D93" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E93" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F93" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="n" s="10">
-        <v>8.0</v>
-      </c>
-      <c r="B94" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="C94" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D94" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="E94" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F94" t="s" s="6">
-        <v>2</v>
+      <c r="A94" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B94" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C94" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D94" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E94" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F94" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n" s="10">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
       <c r="B95" t="s" s="7">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C95" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D95" t="s" s="7">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="E95" t="s" s="6">
         <v>2</v>
@@ -2161,16 +2120,16 @@
     </row>
     <row r="96">
       <c r="A96" t="n" s="10">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
       <c r="B96" t="s" s="7">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C96" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D96" t="s" s="7">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="E96" t="s" s="6">
         <v>2</v>
@@ -2181,16 +2140,16 @@
     </row>
     <row r="97">
       <c r="A97" t="n" s="10">
-        <v>11.0</v>
+        <v>3.0</v>
       </c>
       <c r="B97" t="s" s="7">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C97" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D97" t="s" s="7">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="E97" t="s" s="6">
         <v>2</v>
@@ -2199,100 +2158,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98"/>
-    <row r="99"/>
+    <row r="98">
+      <c r="A98" t="n" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="B98" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="C98" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D98" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="E98" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F98" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="B99" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="C99" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="E99" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F99" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="100">
-      <c r="A100" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B100" t="s" s="4">
-        <v>74</v>
-      </c>
-      <c r="C100" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D100" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E100" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F100" t="s" s="4">
+      <c r="A100" t="n" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="B100" t="s" s="7">
+        <v>60</v>
+      </c>
+      <c r="C100" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D100" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="E100" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F100" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B101" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C101" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D101" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E101" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F101" t="s" s="9">
+      <c r="A101" t="n" s="10">
+        <v>7.0</v>
+      </c>
+      <c r="B101" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="C101" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="E101" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F101" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B102" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C102" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D102" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E102" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F102" t="s" s="8">
+      <c r="A102" t="n" s="10">
+        <v>8.0</v>
+      </c>
+      <c r="B102" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="C102" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="E102" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F102" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B103" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C103" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D103" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E103" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F103" t="s" s="5">
-        <v>25</v>
+      <c r="A103" t="n" s="10">
+        <v>9.0</v>
+      </c>
+      <c r="B103" t="s" s="7">
+        <v>44</v>
+      </c>
+      <c r="C103" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D103" t="s" s="7">
+        <v>45</v>
+      </c>
+      <c r="E103" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F103" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n" s="10">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="B104" t="s" s="7">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C104" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D104" t="s" s="7">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E104" t="s" s="6">
         <v>2</v>
@@ -2303,16 +2300,16 @@
     </row>
     <row r="105">
       <c r="A105" t="n" s="10">
-        <v>2.0</v>
+        <v>11.0</v>
       </c>
       <c r="B105" t="s" s="7">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="C105" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D105" t="s" s="7">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E105" t="s" s="6">
         <v>2</v>
@@ -2333,10 +2330,10 @@
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B65:D65"/>
     <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="B85:F85"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B74:F74"/>
+    <mergeCell ref="B92:D92"/>
+    <mergeCell ref="B93:F93"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
From v1.0.3 to v1.1
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
+++ b/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="75">
   <si>
     <t xml:space="preserve">System: </t>
   </si>
@@ -128,75 +128,75 @@
     <t>SYSTEM Exibe a opcao escolhida: periodo de afastamento.</t>
   </si>
   <si>
+    <t>Chefe/Beneficiário Informa as datas de afastamento, apos o ultimo dia de viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: pernoite.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Detalha a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe os beneficiarios selecionados.</t>
+  </si>
+  <si>
+    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Clica em confirmar.</t>
+  </si>
+  <si>
+    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado.</t>
+  </si>
+  <si>
+    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>O sistema salva os dados</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
+  </si>
+  <si>
     <t>Chefe/Beneficiário Informa as datas de afastamento, antes do ultimo dia de viagem.</t>
   </si>
   <si>
-    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: pernoite.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Detalha a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe os beneficiarios selecionados.</t>
-  </si>
-  <si>
-    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Clica em confirmar.</t>
-  </si>
-  <si>
-    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado.</t>
-  </si>
-  <si>
-    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>O sistema salva os dados</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa as datas de afastamento, apos o ultimo dia de viagem.</t>
-  </si>
-  <si>
     <t>Chefe/Beneficiário Clica em limpar campos.</t>
   </si>
   <si>
@@ -224,19 +224,19 @@
     <t>TC4</t>
   </si>
   <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG202 - RGP Core indisponível.</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
+  </si>
+  <si>
+    <t>TC6</t>
+  </si>
+  <si>
     <t>SYSTEM Exibe a mensagem de erro MSG201 - DNE indisponível.</t>
-  </si>
-  <si>
-    <t>TC5</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
-  </si>
-  <si>
-    <t>TC6</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG202 - RGP Core indisponível.</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="false"/>
   </sheetViews>
@@ -1665,7 +1665,7 @@
         <v>2</v>
       </c>
       <c r="D69" t="s" s="7">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E69" t="s" s="6">
         <v>2</v>
@@ -1674,100 +1674,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70"/>
-    <row r="71"/>
+    <row r="70">
+      <c r="A70" t="n" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="B70" t="s" s="7">
+        <v>30</v>
+      </c>
+      <c r="C70" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D70" t="s" s="7">
+        <v>31</v>
+      </c>
+      <c r="E70" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F70" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="B71" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="C71" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D71" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="E71" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F71" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="72">
-      <c r="A72" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B72" t="s" s="4">
-        <v>71</v>
-      </c>
-      <c r="C72" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D72" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E72" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F72" t="s" s="4">
+      <c r="A72" t="n" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="B72" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="C72" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D72" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="E72" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F72" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B73" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C73" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D73" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E73" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F73" t="s" s="9">
+      <c r="A73" t="n" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="B73" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="C73" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D73" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="E73" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F73" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B74" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C74" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D74" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E74" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F74" t="s" s="8">
+      <c r="A74" t="n" s="10">
+        <v>7.0</v>
+      </c>
+      <c r="B74" t="s" s="7">
+        <v>60</v>
+      </c>
+      <c r="C74" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D74" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="E74" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F74" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B75" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C75" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D75" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E75" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F75" t="s" s="5">
-        <v>25</v>
+      <c r="A75" t="n" s="10">
+        <v>8.0</v>
+      </c>
+      <c r="B75" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="C75" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D75" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="E75" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F75" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n" s="10">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="B76" t="s" s="7">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C76" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D76" t="s" s="7">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="E76" t="s" s="6">
         <v>2</v>
@@ -1778,16 +1816,16 @@
     </row>
     <row r="77">
       <c r="A77" t="n" s="10">
-        <v>2.0</v>
+        <v>10.0</v>
       </c>
       <c r="B77" t="s" s="7">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C77" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D77" t="s" s="7">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="E77" t="s" s="6">
         <v>2</v>
@@ -1798,16 +1836,16 @@
     </row>
     <row r="78">
       <c r="A78" t="n" s="10">
-        <v>3.0</v>
+        <v>11.0</v>
       </c>
       <c r="B78" t="s" s="7">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="C78" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D78" t="s" s="7">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="E78" t="s" s="6">
         <v>2</v>
@@ -1818,16 +1856,16 @@
     </row>
     <row r="79">
       <c r="A79" t="n" s="10">
-        <v>4.0</v>
+        <v>12.0</v>
       </c>
       <c r="B79" t="s" s="7">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C79" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D79" t="s" s="7">
-        <v>33</v>
+        <v>70</v>
       </c>
       <c r="E79" t="s" s="6">
         <v>2</v>
@@ -1836,138 +1874,100 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" t="n" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="B80" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="C80" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D80" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="E80" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F80" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="n" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="B81" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="C81" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D81" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="E81" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F81" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="80"/>
+    <row r="81"/>
     <row r="82">
-      <c r="A82" t="n" s="10">
-        <v>7.0</v>
-      </c>
-      <c r="B82" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="C82" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D82" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="E82" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F82" t="s" s="6">
+      <c r="A82" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B82" t="s" s="4">
+        <v>71</v>
+      </c>
+      <c r="C82" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D82" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E82" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F82" t="s" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="n" s="10">
-        <v>8.0</v>
-      </c>
-      <c r="B83" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="C83" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D83" t="s" s="7">
-        <v>41</v>
-      </c>
-      <c r="E83" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F83" t="s" s="6">
+      <c r="A83" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B83" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D83" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E83" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F83" t="s" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="n" s="10">
-        <v>9.0</v>
-      </c>
-      <c r="B84" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="C84" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D84" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="E84" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F84" t="s" s="6">
+      <c r="A84" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B84" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C84" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E84" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F84" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="n" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="B85" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C85" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D85" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="E85" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F85" t="s" s="6">
-        <v>2</v>
+      <c r="A85" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B85" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C85" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D85" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E85" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F85" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n" s="10">
-        <v>11.0</v>
+        <v>1.0</v>
       </c>
       <c r="B86" t="s" s="7">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C86" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D86" t="s" s="7">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="E86" t="s" s="6">
         <v>2</v>
@@ -1978,16 +1978,16 @@
     </row>
     <row r="87">
       <c r="A87" t="n" s="10">
-        <v>12.0</v>
+        <v>2.0</v>
       </c>
       <c r="B87" t="s" s="7">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="C87" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D87" t="s" s="7">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="E87" t="s" s="6">
         <v>2</v>
@@ -1998,16 +1998,16 @@
     </row>
     <row r="88">
       <c r="A88" t="n" s="10">
-        <v>13.0</v>
+        <v>3.0</v>
       </c>
       <c r="B88" t="s" s="7">
-        <v>49</v>
+        <v>30</v>
       </c>
       <c r="C88" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D88" t="s" s="7">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="E88" t="s" s="6">
         <v>2</v>
@@ -2016,100 +2016,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="89"/>
-    <row r="90"/>
+    <row r="89">
+      <c r="A89" t="n" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="B89" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="C89" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D89" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="E89" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F89" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="B90" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="C90" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D90" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="E90" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F90" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="91">
-      <c r="A91" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B91" t="s" s="4">
-        <v>73</v>
-      </c>
-      <c r="C91" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D91" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E91" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F91" t="s" s="4">
+      <c r="A91" t="n" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="B91" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="C91" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D91" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="E91" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F91" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B92" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C92" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D92" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E92" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F92" t="s" s="9">
+      <c r="A92" t="n" s="10">
+        <v>7.0</v>
+      </c>
+      <c r="B92" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="C92" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D92" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="E92" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F92" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B93" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C93" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D93" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E93" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F93" t="s" s="8">
+      <c r="A93" t="n" s="10">
+        <v>8.0</v>
+      </c>
+      <c r="B93" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="C93" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D93" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="E93" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F93" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B94" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C94" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D94" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E94" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F94" t="s" s="5">
-        <v>25</v>
+      <c r="A94" t="n" s="10">
+        <v>9.0</v>
+      </c>
+      <c r="B94" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="C94" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D94" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="E94" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F94" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n" s="10">
-        <v>1.0</v>
+        <v>10.0</v>
       </c>
       <c r="B95" t="s" s="7">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C95" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D95" t="s" s="7">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="E95" t="s" s="6">
         <v>2</v>
@@ -2120,16 +2158,16 @@
     </row>
     <row r="96">
       <c r="A96" t="n" s="10">
-        <v>2.0</v>
+        <v>11.0</v>
       </c>
       <c r="B96" t="s" s="7">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C96" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D96" t="s" s="7">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E96" t="s" s="6">
         <v>2</v>
@@ -2140,16 +2178,16 @@
     </row>
     <row r="97">
       <c r="A97" t="n" s="10">
-        <v>3.0</v>
+        <v>12.0</v>
       </c>
       <c r="B97" t="s" s="7">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C97" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D97" t="s" s="7">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="E97" t="s" s="6">
         <v>2</v>
@@ -2160,16 +2198,16 @@
     </row>
     <row r="98">
       <c r="A98" t="n" s="10">
-        <v>4.0</v>
+        <v>13.0</v>
       </c>
       <c r="B98" t="s" s="7">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C98" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D98" t="s" s="7">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="E98" t="s" s="6">
         <v>2</v>
@@ -2178,143 +2216,125 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" t="n" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="B99" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="C99" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D99" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="E99" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F99" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="n" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="B100" t="s" s="7">
-        <v>60</v>
-      </c>
-      <c r="C100" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D100" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="E100" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F100" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="99"/>
+    <row r="100"/>
     <row r="101">
-      <c r="A101" t="n" s="10">
-        <v>7.0</v>
-      </c>
-      <c r="B101" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="C101" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D101" t="s" s="7">
-        <v>41</v>
-      </c>
-      <c r="E101" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F101" t="s" s="6">
+      <c r="A101" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B101" t="s" s="4">
+        <v>73</v>
+      </c>
+      <c r="C101" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D101" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E101" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F101" t="s" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="n" s="10">
-        <v>8.0</v>
-      </c>
-      <c r="B102" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="C102" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D102" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="E102" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F102" t="s" s="6">
+      <c r="A102" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B102" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C102" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E102" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F102" t="s" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="n" s="10">
-        <v>9.0</v>
-      </c>
-      <c r="B103" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C103" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D103" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="E103" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F103" t="s" s="6">
+      <c r="A103" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B103" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C103" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D103" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E103" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F103" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="n" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="B104" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C104" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D104" t="s" s="7">
-        <v>47</v>
-      </c>
-      <c r="E104" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F104" t="s" s="6">
-        <v>2</v>
+      <c r="A104" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B104" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C104" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D104" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E104" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F104" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n" s="10">
-        <v>11.0</v>
+        <v>1.0</v>
       </c>
       <c r="B105" t="s" s="7">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="C105" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D105" t="s" s="7">
+        <v>65</v>
+      </c>
+      <c r="E105" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F105" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="B106" t="s" s="7">
+        <v>66</v>
+      </c>
+      <c r="C106" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D106" t="s" s="7">
         <v>74</v>
       </c>
-      <c r="E105" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F105" t="s" s="6">
+      <c r="E106" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F106" t="s" s="6">
         <v>2</v>
       </c>
     </row>
@@ -2330,10 +2350,10 @@
     <mergeCell ref="B47:F47"/>
     <mergeCell ref="B65:D65"/>
     <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B74:F74"/>
-    <mergeCell ref="B92:D92"/>
-    <mergeCell ref="B93:F93"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B102:D102"/>
+    <mergeCell ref="B103:F103"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
From v1.1 to v1.1.1
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
+++ b/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="75">
   <si>
     <t xml:space="preserve">System: </t>
   </si>
@@ -128,75 +128,75 @@
     <t>SYSTEM Exibe a opcao escolhida: periodo de afastamento.</t>
   </si>
   <si>
+    <t>Chefe/Beneficiário Informa as datas de afastamento, antes do ultimo dia de viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: pernoite.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Detalha a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe os beneficiarios selecionados.</t>
+  </si>
+  <si>
+    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Clica em confirmar.</t>
+  </si>
+  <si>
+    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado. 3. Manutenção do cargo comissionado e do setor beneficiário à época da concessão da diária.</t>
+  </si>
+  <si>
+    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>O sistema salva os dados</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
+  </si>
+  <si>
     <t>Chefe/Beneficiário Informa as datas de afastamento, apos o ultimo dia de viagem.</t>
   </si>
   <si>
-    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: pernoite.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Detalha a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe os beneficiarios selecionados.</t>
-  </si>
-  <si>
-    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Clica em confirmar.</t>
-  </si>
-  <si>
-    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado.</t>
-  </si>
-  <si>
-    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>O sistema salva os dados</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa as datas de afastamento, antes do ultimo dia de viagem.</t>
-  </si>
-  <si>
     <t>Chefe/Beneficiário Clica em limpar campos.</t>
   </si>
   <si>
@@ -218,13 +218,13 @@
     <t>SYSTEM Exibe a opcao escolhida: estado.</t>
   </si>
   <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG202 - RGP Core indisponível.</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
     <t>SYSTEM Exibe a mensagem de erro MSG203 - Campos obrigatórios, MSG214 - Campos obrigatórios da solicitação de diárias (não informados).</t>
-  </si>
-  <si>
-    <t>TC4</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG202 - RGP Core indisponível.</t>
   </si>
   <si>
     <t>TC5</t>
@@ -432,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:F105"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="false"/>
   </sheetViews>
@@ -1523,7 +1523,7 @@
         <v>2</v>
       </c>
       <c r="D60" t="s" s="7">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="E60" t="s" s="6">
         <v>2</v>
@@ -1532,120 +1532,120 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="n" s="10">
-        <v>13.0</v>
-      </c>
-      <c r="B61" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="C61" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D61" t="s" s="7">
-        <v>68</v>
-      </c>
-      <c r="E61" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F61" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="61"/>
     <row r="62"/>
-    <row r="63"/>
+    <row r="63">
+      <c r="A63" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B63" t="s" s="4">
+        <v>69</v>
+      </c>
+      <c r="C63" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D63" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E63" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F63" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
     <row r="64">
-      <c r="A64" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B64" t="s" s="4">
-        <v>69</v>
-      </c>
-      <c r="C64" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D64" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E64" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F64" t="s" s="4">
+      <c r="A64" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B64" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F64" t="s" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B65" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C65" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D65" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E65" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F65" t="s" s="9">
+      <c r="A65" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B65" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C65" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F65" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B66" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C66" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D66" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E66" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F66" t="s" s="8">
-        <v>2</v>
+      <c r="A66" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B66" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C66" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D66" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E66" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F66" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B67" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C67" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D67" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E67" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F67" t="s" s="5">
-        <v>25</v>
+      <c r="A67" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B67" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="C67" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s" s="7">
+        <v>65</v>
+      </c>
+      <c r="E67" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F67" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n" s="10">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B68" t="s" s="7">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C68" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D68" t="s" s="7">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E68" t="s" s="6">
         <v>2</v>
@@ -1656,16 +1656,16 @@
     </row>
     <row r="69">
       <c r="A69" t="n" s="10">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B69" t="s" s="7">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="C69" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D69" t="s" s="7">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="E69" t="s" s="6">
         <v>2</v>
@@ -1676,16 +1676,16 @@
     </row>
     <row r="70">
       <c r="A70" t="n" s="10">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B70" t="s" s="7">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C70" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D70" t="s" s="7">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E70" t="s" s="6">
         <v>2</v>
@@ -1696,16 +1696,16 @@
     </row>
     <row r="71">
       <c r="A71" t="n" s="10">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="B71" t="s" s="7">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C71" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D71" t="s" s="7">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E71" t="s" s="6">
         <v>2</v>
@@ -1716,16 +1716,16 @@
     </row>
     <row r="72">
       <c r="A72" t="n" s="10">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="B72" t="s" s="7">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C72" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D72" t="s" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E72" t="s" s="6">
         <v>2</v>
@@ -1736,16 +1736,16 @@
     </row>
     <row r="73">
       <c r="A73" t="n" s="10">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="B73" t="s" s="7">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C73" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D73" t="s" s="7">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E73" t="s" s="6">
         <v>2</v>
@@ -1756,16 +1756,16 @@
     </row>
     <row r="74">
       <c r="A74" t="n" s="10">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="B74" t="s" s="7">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="C74" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D74" t="s" s="7">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E74" t="s" s="6">
         <v>2</v>
@@ -1776,16 +1776,16 @@
     </row>
     <row r="75">
       <c r="A75" t="n" s="10">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="B75" t="s" s="7">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C75" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D75" t="s" s="7">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E75" t="s" s="6">
         <v>2</v>
@@ -1796,16 +1796,16 @@
     </row>
     <row r="76">
       <c r="A76" t="n" s="10">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="B76" t="s" s="7">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C76" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D76" t="s" s="7">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E76" t="s" s="6">
         <v>2</v>
@@ -1816,16 +1816,16 @@
     </row>
     <row r="77">
       <c r="A77" t="n" s="10">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="B77" t="s" s="7">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C77" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D77" t="s" s="7">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E77" t="s" s="6">
         <v>2</v>
@@ -1836,7 +1836,7 @@
     </row>
     <row r="78">
       <c r="A78" t="n" s="10">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="B78" t="s" s="7">
         <v>46</v>
@@ -1845,7 +1845,7 @@
         <v>2</v>
       </c>
       <c r="D78" t="s" s="7">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E78" t="s" s="6">
         <v>2</v>
@@ -1856,10 +1856,10 @@
     </row>
     <row r="79">
       <c r="A79" t="n" s="10">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
       <c r="B79" t="s" s="7">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C79" t="s" s="6">
         <v>2</v>
@@ -1961,13 +1961,13 @@
         <v>1.0</v>
       </c>
       <c r="B86" t="s" s="7">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C86" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D86" t="s" s="7">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E86" t="s" s="6">
         <v>2</v>
@@ -1981,13 +1981,13 @@
         <v>2.0</v>
       </c>
       <c r="B87" t="s" s="7">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C87" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D87" t="s" s="7">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E87" t="s" s="6">
         <v>2</v>
@@ -2001,13 +2001,13 @@
         <v>3.0</v>
       </c>
       <c r="B88" t="s" s="7">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C88" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D88" t="s" s="7">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E88" t="s" s="6">
         <v>2</v>
@@ -2021,13 +2021,13 @@
         <v>4.0</v>
       </c>
       <c r="B89" t="s" s="7">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C89" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D89" t="s" s="7">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E89" t="s" s="6">
         <v>2</v>
@@ -2041,13 +2041,13 @@
         <v>5.0</v>
       </c>
       <c r="B90" t="s" s="7">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C90" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D90" t="s" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E90" t="s" s="6">
         <v>2</v>
@@ -2061,13 +2061,13 @@
         <v>6.0</v>
       </c>
       <c r="B91" t="s" s="7">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C91" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D91" t="s" s="7">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E91" t="s" s="6">
         <v>2</v>
@@ -2081,13 +2081,13 @@
         <v>7.0</v>
       </c>
       <c r="B92" t="s" s="7">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C92" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D92" t="s" s="7">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E92" t="s" s="6">
         <v>2</v>
@@ -2101,13 +2101,13 @@
         <v>8.0</v>
       </c>
       <c r="B93" t="s" s="7">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C93" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D93" t="s" s="7">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E93" t="s" s="6">
         <v>2</v>
@@ -2121,13 +2121,13 @@
         <v>9.0</v>
       </c>
       <c r="B94" t="s" s="7">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C94" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D94" t="s" s="7">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E94" t="s" s="6">
         <v>2</v>
@@ -2141,13 +2141,13 @@
         <v>10.0</v>
       </c>
       <c r="B95" t="s" s="7">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C95" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D95" t="s" s="7">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E95" t="s" s="6">
         <v>2</v>
@@ -2167,7 +2167,7 @@
         <v>2</v>
       </c>
       <c r="D96" t="s" s="7">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E96" t="s" s="6">
         <v>2</v>
@@ -2181,13 +2181,13 @@
         <v>12.0</v>
       </c>
       <c r="B97" t="s" s="7">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C97" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D97" t="s" s="7">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="E97" t="s" s="6">
         <v>2</v>
@@ -2196,145 +2196,125 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" t="n" s="10">
-        <v>13.0</v>
-      </c>
-      <c r="B98" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="C98" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D98" t="s" s="7">
-        <v>72</v>
-      </c>
-      <c r="E98" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F98" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="98"/>
     <row r="99"/>
-    <row r="100"/>
+    <row r="100">
+      <c r="A100" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B100" t="s" s="4">
+        <v>73</v>
+      </c>
+      <c r="C100" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D100" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E100" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F100" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
     <row r="101">
-      <c r="A101" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B101" t="s" s="4">
-        <v>73</v>
-      </c>
-      <c r="C101" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D101" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E101" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F101" t="s" s="4">
+      <c r="A101" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B101" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C101" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E101" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F101" t="s" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B102" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C102" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D102" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E102" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F102" t="s" s="9">
+      <c r="A102" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B102" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C102" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E102" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F102" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B103" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C103" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D103" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E103" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F103" t="s" s="8">
-        <v>2</v>
+      <c r="A103" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B103" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C103" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D103" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E103" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F103" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B104" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C104" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D104" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E104" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F104" t="s" s="5">
-        <v>25</v>
+      <c r="A104" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B104" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="C104" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D104" t="s" s="7">
+        <v>65</v>
+      </c>
+      <c r="E104" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F104" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n" s="10">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B105" t="s" s="7">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C105" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D105" t="s" s="7">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="E105" t="s" s="6">
         <v>2</v>
       </c>
       <c r="F105" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="n" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="B106" t="s" s="7">
-        <v>66</v>
-      </c>
-      <c r="C106" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D106" t="s" s="7">
-        <v>74</v>
-      </c>
-      <c r="E106" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F106" t="s" s="6">
         <v>2</v>
       </c>
     </row>
@@ -2348,12 +2328,12 @@
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:F65"/>
     <mergeCell ref="B83:D83"/>
     <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B102:D102"/>
-    <mergeCell ref="B103:F103"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B102:F102"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
From v1.1.1 to v1.2
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
+++ b/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="77">
   <si>
     <t xml:space="preserve">System: </t>
   </si>
@@ -41,7 +41,7 @@
     <t>Reduced (Greedy Heuristic - Transition Coverage)</t>
   </si>
   <si>
-    <t>Size: 6 test case(s))</t>
+    <t>Size: 7 test case(s))</t>
   </si>
   <si>
     <t xml:space="preserve">Creation Date: </t>
@@ -218,22 +218,28 @@
     <t>SYSTEM Exibe a opcao escolhida: estado.</t>
   </si>
   <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>SYSTEM Não confirma a existencia de conta para recebimento de diarias do servidor. Exibe a mensagem de erro MSG002 - Conta para recebimento de diárias não cadastrada.</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG203 - Campos obrigatórios, MSG214 - Campos obrigatórios da solicitação de diárias (não informados).</t>
+  </si>
+  <si>
+    <t>TC6</t>
+  </si>
+  <si>
     <t>SYSTEM Exibe a mensagem de erro MSG202 - RGP Core indisponível.</t>
   </si>
   <si>
-    <t>TC4</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG203 - Campos obrigatórios, MSG214 - Campos obrigatórios da solicitação de diárias (não informados).</t>
-  </si>
-  <si>
-    <t>TC5</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
-  </si>
-  <si>
-    <t>TC6</t>
+    <t>TC7</t>
   </si>
   <si>
     <t>SYSTEM Exibe a mensagem de erro MSG201 - DNE indisponível.</t>
@@ -432,7 +438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F105"/>
+  <dimension ref="A1:F120"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="false"/>
   </sheetViews>
@@ -1523,129 +1529,129 @@
         <v>2</v>
       </c>
       <c r="D60" t="s" s="7">
+        <v>48</v>
+      </c>
+      <c r="E60" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F60" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n" s="10">
+        <v>13.0</v>
+      </c>
+      <c r="B61" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="C61" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D61" t="s" s="7">
         <v>68</v>
       </c>
-      <c r="E60" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F60" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="61"/>
+      <c r="E61" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F61" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="62"/>
-    <row r="63">
-      <c r="A63" t="s" s="4">
+    <row r="63"/>
+    <row r="64">
+      <c r="A64" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B63" t="s" s="4">
+      <c r="B64" t="s" s="4">
         <v>69</v>
       </c>
-      <c r="C63" t="s" s="4">
+      <c r="C64" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D63" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E63" t="s" s="4">
+      <c r="D64" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F63" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s" s="9">
+      <c r="F64" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E64" t="s" s="9">
+      <c r="B65" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C65" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F64" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s" s="8">
+      <c r="F65" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B65" t="s" s="8">
+      <c r="B66" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F65" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s" s="5">
+      <c r="C66" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E66" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F66" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B66" t="s" s="5">
+      <c r="B67" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C66" t="s" s="5">
+      <c r="C67" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D66" t="s" s="5">
+      <c r="D67" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E66" t="s" s="5">
+      <c r="E67" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F66" t="s" s="5">
+      <c r="F67" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B67" t="s" s="7">
-        <v>64</v>
-      </c>
-      <c r="C67" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D67" t="s" s="7">
-        <v>65</v>
-      </c>
-      <c r="E67" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F67" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n" s="10">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B68" t="s" s="7">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C68" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D68" t="s" s="7">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E68" t="s" s="6">
         <v>2</v>
@@ -1656,16 +1662,16 @@
     </row>
     <row r="69">
       <c r="A69" t="n" s="10">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B69" t="s" s="7">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="C69" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D69" t="s" s="7">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="E69" t="s" s="6">
         <v>2</v>
@@ -1676,7 +1682,7 @@
     </row>
     <row r="70">
       <c r="A70" t="n" s="10">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B70" t="s" s="7">
         <v>32</v>
@@ -1696,7 +1702,7 @@
     </row>
     <row r="71">
       <c r="A71" t="n" s="10">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B71" t="s" s="7">
         <v>34</v>
@@ -1716,7 +1722,7 @@
     </row>
     <row r="72">
       <c r="A72" t="n" s="10">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B72" t="s" s="7">
         <v>36</v>
@@ -1736,7 +1742,7 @@
     </row>
     <row r="73">
       <c r="A73" t="n" s="10">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B73" t="s" s="7">
         <v>60</v>
@@ -1756,7 +1762,7 @@
     </row>
     <row r="74">
       <c r="A74" t="n" s="10">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B74" t="s" s="7">
         <v>40</v>
@@ -1776,7 +1782,7 @@
     </row>
     <row r="75">
       <c r="A75" t="n" s="10">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B75" t="s" s="7">
         <v>42</v>
@@ -1796,7 +1802,7 @@
     </row>
     <row r="76">
       <c r="A76" t="n" s="10">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="B76" t="s" s="7">
         <v>44</v>
@@ -1816,7 +1822,7 @@
     </row>
     <row r="77">
       <c r="A77" t="n" s="10">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="B77" t="s" s="7">
         <v>46</v>
@@ -1825,7 +1831,7 @@
         <v>2</v>
       </c>
       <c r="D77" t="s" s="7">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="E77" t="s" s="6">
         <v>2</v>
@@ -1834,140 +1840,140 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" t="n" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B78" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C78" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D78" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="E78" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F78" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n" s="10">
-        <v>13.0</v>
-      </c>
-      <c r="B79" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="C79" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D79" t="s" s="7">
-        <v>70</v>
-      </c>
-      <c r="E79" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F79" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80"/>
-    <row r="81"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80">
+      <c r="A80" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B80" t="s" s="4">
+        <v>71</v>
+      </c>
+      <c r="C80" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D80" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E80" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F80" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B81" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E81" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F81" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
     <row r="82">
-      <c r="A82" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B82" t="s" s="4">
-        <v>71</v>
-      </c>
-      <c r="C82" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D82" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E82" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F82" t="s" s="4">
+      <c r="A82" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B82" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C82" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E82" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F82" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B83" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C83" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D83" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E83" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F83" t="s" s="9">
-        <v>2</v>
+      <c r="A83" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B83" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C83" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D83" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E83" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F83" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B84" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C84" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D84" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E84" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F84" t="s" s="8">
+      <c r="A84" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B84" t="s" s="7">
+        <v>56</v>
+      </c>
+      <c r="C84" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s" s="7">
+        <v>57</v>
+      </c>
+      <c r="E84" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F84" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B85" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C85" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D85" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E85" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F85" t="s" s="5">
-        <v>25</v>
+      <c r="A85" t="n" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="B85" t="s" s="7">
+        <v>58</v>
+      </c>
+      <c r="C85" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D85" t="s" s="7">
+        <v>59</v>
+      </c>
+      <c r="E85" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F85" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n" s="10">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B86" t="s" s="7">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C86" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D86" t="s" s="7">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="E86" t="s" s="6">
         <v>2</v>
@@ -1978,16 +1984,16 @@
     </row>
     <row r="87">
       <c r="A87" t="n" s="10">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B87" t="s" s="7">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C87" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D87" t="s" s="7">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="E87" t="s" s="6">
         <v>2</v>
@@ -1998,16 +2004,16 @@
     </row>
     <row r="88">
       <c r="A88" t="n" s="10">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="B88" t="s" s="7">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C88" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D88" t="s" s="7">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E88" t="s" s="6">
         <v>2</v>
@@ -2018,16 +2024,16 @@
     </row>
     <row r="89">
       <c r="A89" t="n" s="10">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="B89" t="s" s="7">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C89" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D89" t="s" s="7">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E89" t="s" s="6">
         <v>2</v>
@@ -2038,16 +2044,16 @@
     </row>
     <row r="90">
       <c r="A90" t="n" s="10">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="B90" t="s" s="7">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C90" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D90" t="s" s="7">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E90" t="s" s="6">
         <v>2</v>
@@ -2058,16 +2064,16 @@
     </row>
     <row r="91">
       <c r="A91" t="n" s="10">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="B91" t="s" s="7">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C91" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D91" t="s" s="7">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E91" t="s" s="6">
         <v>2</v>
@@ -2078,16 +2084,16 @@
     </row>
     <row r="92">
       <c r="A92" t="n" s="10">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="B92" t="s" s="7">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C92" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D92" t="s" s="7">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E92" t="s" s="6">
         <v>2</v>
@@ -2098,16 +2104,16 @@
     </row>
     <row r="93">
       <c r="A93" t="n" s="10">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="B93" t="s" s="7">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C93" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D93" t="s" s="7">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E93" t="s" s="6">
         <v>2</v>
@@ -2118,16 +2124,16 @@
     </row>
     <row r="94">
       <c r="A94" t="n" s="10">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="B94" t="s" s="7">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C94" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D94" t="s" s="7">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E94" t="s" s="6">
         <v>2</v>
@@ -2138,16 +2144,16 @@
     </row>
     <row r="95">
       <c r="A95" t="n" s="10">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="B95" t="s" s="7">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C95" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D95" t="s" s="7">
-        <v>47</v>
+        <v>72</v>
       </c>
       <c r="E95" t="s" s="6">
         <v>2</v>
@@ -2156,140 +2162,140 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" t="n" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="B96" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C96" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D96" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="E96" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F96" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B97" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="C97" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D97" t="s" s="7">
-        <v>72</v>
-      </c>
-      <c r="E97" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F97" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98"/>
-    <row r="99"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98">
+      <c r="A98" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B98" t="s" s="4">
+        <v>73</v>
+      </c>
+      <c r="C98" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D98" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E98" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F98" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B99" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E99" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F99" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
     <row r="100">
-      <c r="A100" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B100" t="s" s="4">
-        <v>73</v>
-      </c>
-      <c r="C100" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D100" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E100" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F100" t="s" s="4">
+      <c r="A100" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B100" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C100" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D100" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E100" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F100" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B101" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C101" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D101" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E101" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F101" t="s" s="9">
-        <v>2</v>
+      <c r="A101" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B101" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C101" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D101" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E101" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F101" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B102" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C102" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D102" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E102" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F102" t="s" s="8">
+      <c r="A102" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B102" t="s" s="7">
+        <v>56</v>
+      </c>
+      <c r="C102" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s" s="7">
+        <v>57</v>
+      </c>
+      <c r="E102" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F102" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B103" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C103" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D103" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E103" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F103" t="s" s="5">
-        <v>25</v>
+      <c r="A103" t="n" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="B103" t="s" s="7">
+        <v>58</v>
+      </c>
+      <c r="C103" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D103" t="s" s="7">
+        <v>59</v>
+      </c>
+      <c r="E103" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F103" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n" s="10">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B104" t="s" s="7">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="C104" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D104" t="s" s="7">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="E104" t="s" s="6">
         <v>2</v>
@@ -2300,21 +2306,283 @@
     </row>
     <row r="105">
       <c r="A105" t="n" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="B105" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="C105" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D105" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="E105" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F105" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="B106" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="C106" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D106" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="E106" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F106" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="B107" t="s" s="7">
+        <v>60</v>
+      </c>
+      <c r="C107" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D107" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="E107" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F107" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n" s="10">
+        <v>7.0</v>
+      </c>
+      <c r="B108" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="C108" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D108" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="E108" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F108" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n" s="10">
+        <v>8.0</v>
+      </c>
+      <c r="B109" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="C109" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D109" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="E109" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F109" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n" s="10">
+        <v>9.0</v>
+      </c>
+      <c r="B110" t="s" s="7">
+        <v>44</v>
+      </c>
+      <c r="C110" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D110" t="s" s="7">
+        <v>45</v>
+      </c>
+      <c r="E110" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F110" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="B111" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C111" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D111" t="s" s="7">
+        <v>47</v>
+      </c>
+      <c r="E111" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F111" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n" s="10">
+        <v>11.0</v>
+      </c>
+      <c r="B112" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C112" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D112" t="s" s="7">
+        <v>74</v>
+      </c>
+      <c r="E112" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F112" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113"/>
+    <row r="114"/>
+    <row r="115">
+      <c r="A115" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B115" t="s" s="4">
+        <v>75</v>
+      </c>
+      <c r="C115" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D115" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E115" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F115" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B116" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C116" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D116" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E116" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F116" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B117" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C117" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D117" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E117" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F117" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B118" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C118" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D118" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E118" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F118" t="s" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B119" t="s" s="7">
+        <v>64</v>
+      </c>
+      <c r="C119" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D119" t="s" s="7">
+        <v>65</v>
+      </c>
+      <c r="E119" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F119" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n" s="10">
         <v>2.0</v>
       </c>
-      <c r="B105" t="s" s="7">
+      <c r="B120" t="s" s="7">
         <v>66</v>
       </c>
-      <c r="C105" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D105" t="s" s="7">
-        <v>74</v>
-      </c>
-      <c r="E105" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F105" t="s" s="6">
+      <c r="C120" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D120" t="s" s="7">
+        <v>76</v>
+      </c>
+      <c r="E120" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F120" t="s" s="6">
         <v>2</v>
       </c>
     </row>
@@ -2328,12 +2596,14 @@
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B66:F66"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B117:F117"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
From v1.2 to v1.2.1
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
+++ b/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="79">
   <si>
     <t xml:space="preserve">System: </t>
   </si>
@@ -155,48 +155,54 @@
     <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
   </si>
   <si>
+    <t>SYSTEM Exibe os beneficiarios selecionados e o campo para preenchimento do nome social</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa o nome social do beneficiario da(s) diaria(s)</t>
+  </si>
+  <si>
+    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Clica em confirmar.</t>
+  </si>
+  <si>
+    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado. 3. Manutenção do cargo comissionado e do setor beneficiário à época da concessão da diária.</t>
+  </si>
+  <si>
+    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>O sistema salva os dados</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa as datas de afastamento, apos o ultimo dia de viagem.</t>
+  </si>
+  <si>
     <t>SYSTEM Exibe os beneficiarios selecionados.</t>
   </si>
   <si>
-    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Clica em confirmar.</t>
-  </si>
-  <si>
-    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado. 3. Manutenção do cargo comissionado e do setor beneficiário à época da concessão da diária.</t>
-  </si>
-  <si>
-    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>O sistema salva os dados</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa as datas de afastamento, apos o ultimo dia de viagem.</t>
-  </si>
-  <si>
     <t>Chefe/Beneficiário Clica em limpar campos.</t>
   </si>
   <si>
@@ -218,31 +224,31 @@
     <t>SYSTEM Exibe a opcao escolhida: estado.</t>
   </si>
   <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG202 - RGP Core indisponível.</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG203 - Campos obrigatórios, MSG214 - Campos obrigatórios da solicitação de diárias (não informados).</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
     <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
   </si>
   <si>
-    <t>TC4</t>
+    <t>TC6</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG201 - DNE indisponível.</t>
+  </si>
+  <si>
+    <t>TC7</t>
   </si>
   <si>
     <t>SYSTEM Não confirma a existencia de conta para recebimento de diarias do servidor. Exibe a mensagem de erro MSG002 - Conta para recebimento de diárias não cadastrada.</t>
-  </si>
-  <si>
-    <t>TC5</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG203 - Campos obrigatórios, MSG214 - Campos obrigatórios da solicitação de diárias (não informados).</t>
-  </si>
-  <si>
-    <t>TC6</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG202 - RGP Core indisponível.</t>
-  </si>
-  <si>
-    <t>TC7</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG201 - DNE indisponível.</t>
   </si>
 </sst>
 </file>
@@ -438,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F120"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="false"/>
   </sheetViews>
@@ -819,13 +825,13 @@
         <v>12.0</v>
       </c>
       <c r="B21" t="s" s="7">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D21" t="s" s="7">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s" s="6">
         <v>2</v>
@@ -839,13 +845,13 @@
         <v>13.0</v>
       </c>
       <c r="B22" t="s" s="7">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D22" t="s" s="7">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s" s="6">
         <v>2</v>
@@ -859,13 +865,13 @@
         <v>14.0</v>
       </c>
       <c r="B23" t="s" s="7">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D23" t="s" s="7">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E23" t="s" s="6">
         <v>2</v>
@@ -876,10 +882,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s" s="8">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s" s="8">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s" s="8">
         <v>2</v>
@@ -901,7 +907,7 @@
         <v>12</v>
       </c>
       <c r="B27" t="s" s="4">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s" s="4">
         <v>14</v>
@@ -981,13 +987,13 @@
         <v>1.0</v>
       </c>
       <c r="B31" t="s" s="7">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D31" t="s" s="7">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E31" t="s" s="6">
         <v>2</v>
@@ -1001,13 +1007,13 @@
         <v>2.0</v>
       </c>
       <c r="B32" t="s" s="7">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D32" t="s" s="7">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E32" t="s" s="6">
         <v>2</v>
@@ -1081,7 +1087,7 @@
         <v>6.0</v>
       </c>
       <c r="B36" t="s" s="7">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s" s="6">
         <v>2</v>
@@ -1167,7 +1173,7 @@
         <v>2</v>
       </c>
       <c r="D40" t="s" s="7">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="E40" t="s" s="6">
         <v>2</v>
@@ -1187,7 +1193,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s" s="7">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E41" t="s" s="6">
         <v>2</v>
@@ -1201,13 +1207,13 @@
         <v>12.0</v>
       </c>
       <c r="B42" t="s" s="7">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C42" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D42" t="s" s="7">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E42" t="s" s="6">
         <v>2</v>
@@ -1223,7 +1229,7 @@
         <v>12</v>
       </c>
       <c r="B45" t="s" s="4">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C45" t="s" s="4">
         <v>14</v>
@@ -1303,13 +1309,13 @@
         <v>1.0</v>
       </c>
       <c r="B49" t="s" s="7">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C49" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D49" t="s" s="7">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E49" t="s" s="6">
         <v>2</v>
@@ -1323,13 +1329,13 @@
         <v>2.0</v>
       </c>
       <c r="B50" t="s" s="7">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C50" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D50" t="s" s="7">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E50" t="s" s="6">
         <v>2</v>
@@ -1423,7 +1429,7 @@
         <v>7.0</v>
       </c>
       <c r="B55" t="s" s="7">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C55" t="s" s="6">
         <v>2</v>
@@ -1509,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="D59" t="s" s="7">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="E59" t="s" s="6">
         <v>2</v>
@@ -1529,7 +1535,7 @@
         <v>2</v>
       </c>
       <c r="D60" t="s" s="7">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="E60" t="s" s="6">
         <v>2</v>
@@ -1538,120 +1544,120 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61">
-      <c r="A61" t="n" s="10">
-        <v>13.0</v>
-      </c>
-      <c r="B61" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="C61" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D61" t="s" s="7">
-        <v>68</v>
-      </c>
-      <c r="E61" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F61" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="61"/>
     <row r="62"/>
-    <row r="63"/>
+    <row r="63">
+      <c r="A63" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B63" t="s" s="4">
+        <v>71</v>
+      </c>
+      <c r="C63" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D63" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E63" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F63" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
     <row r="64">
-      <c r="A64" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B64" t="s" s="4">
-        <v>69</v>
-      </c>
-      <c r="C64" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D64" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E64" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F64" t="s" s="4">
+      <c r="A64" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B64" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F64" t="s" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B65" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C65" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D65" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E65" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F65" t="s" s="9">
+      <c r="A65" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B65" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C65" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F65" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B66" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C66" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D66" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E66" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F66" t="s" s="8">
-        <v>2</v>
+      <c r="A66" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B66" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C66" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D66" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E66" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F66" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B67" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C67" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D67" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E67" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F67" t="s" s="5">
-        <v>25</v>
+      <c r="A67" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B67" t="s" s="7">
+        <v>66</v>
+      </c>
+      <c r="C67" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s" s="7">
+        <v>67</v>
+      </c>
+      <c r="E67" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F67" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n" s="10">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B68" t="s" s="7">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C68" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D68" t="s" s="7">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="E68" t="s" s="6">
         <v>2</v>
@@ -1662,16 +1668,16 @@
     </row>
     <row r="69">
       <c r="A69" t="n" s="10">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B69" t="s" s="7">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="C69" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D69" t="s" s="7">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="E69" t="s" s="6">
         <v>2</v>
@@ -1682,7 +1688,7 @@
     </row>
     <row r="70">
       <c r="A70" t="n" s="10">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B70" t="s" s="7">
         <v>32</v>
@@ -1702,7 +1708,7 @@
     </row>
     <row r="71">
       <c r="A71" t="n" s="10">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="B71" t="s" s="7">
         <v>34</v>
@@ -1722,7 +1728,7 @@
     </row>
     <row r="72">
       <c r="A72" t="n" s="10">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="B72" t="s" s="7">
         <v>36</v>
@@ -1742,10 +1748,10 @@
     </row>
     <row r="73">
       <c r="A73" t="n" s="10">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="B73" t="s" s="7">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C73" t="s" s="6">
         <v>2</v>
@@ -1762,7 +1768,7 @@
     </row>
     <row r="74">
       <c r="A74" t="n" s="10">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="B74" t="s" s="7">
         <v>40</v>
@@ -1782,7 +1788,7 @@
     </row>
     <row r="75">
       <c r="A75" t="n" s="10">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="B75" t="s" s="7">
         <v>42</v>
@@ -1802,7 +1808,7 @@
     </row>
     <row r="76">
       <c r="A76" t="n" s="10">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="B76" t="s" s="7">
         <v>44</v>
@@ -1822,7 +1828,7 @@
     </row>
     <row r="77">
       <c r="A77" t="n" s="10">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="B77" t="s" s="7">
         <v>46</v>
@@ -1831,7 +1837,7 @@
         <v>2</v>
       </c>
       <c r="D77" t="s" s="7">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E77" t="s" s="6">
         <v>2</v>
@@ -1840,140 +1846,140 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78"/>
-    <row r="79"/>
-    <row r="80">
-      <c r="A80" t="s" s="4">
+    <row r="78">
+      <c r="A78" t="n" s="10">
+        <v>12.0</v>
+      </c>
+      <c r="B78" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C78" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="E78" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F78" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n" s="10">
+        <v>13.0</v>
+      </c>
+      <c r="B79" t="s" s="7">
+        <v>50</v>
+      </c>
+      <c r="C79" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s" s="7">
+        <v>72</v>
+      </c>
+      <c r="E79" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F79" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82">
+      <c r="A82" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B80" t="s" s="4">
-        <v>71</v>
-      </c>
-      <c r="C80" t="s" s="4">
+      <c r="B82" t="s" s="4">
+        <v>73</v>
+      </c>
+      <c r="C82" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D80" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E80" t="s" s="4">
+      <c r="D82" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E82" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F80" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s" s="9">
+      <c r="F82" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B81" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C81" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D81" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E81" t="s" s="9">
+      <c r="B83" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C83" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D83" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E83" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F81" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s" s="8">
+      <c r="F83" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B82" t="s" s="8">
+      <c r="B84" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C82" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D82" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E82" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F82" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s" s="5">
+      <c r="C84" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E84" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F84" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B83" t="s" s="5">
+      <c r="B85" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C83" t="s" s="5">
+      <c r="C85" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D83" t="s" s="5">
+      <c r="D85" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E83" t="s" s="5">
+      <c r="E85" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F83" t="s" s="5">
+      <c r="F85" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B84" t="s" s="7">
-        <v>56</v>
-      </c>
-      <c r="C84" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D84" t="s" s="7">
-        <v>57</v>
-      </c>
-      <c r="E84" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F84" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="n" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="B85" t="s" s="7">
-        <v>58</v>
-      </c>
-      <c r="C85" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D85" t="s" s="7">
-        <v>59</v>
-      </c>
-      <c r="E85" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F85" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n" s="10">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B86" t="s" s="7">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="C86" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D86" t="s" s="7">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="E86" t="s" s="6">
         <v>2</v>
@@ -1984,16 +1990,16 @@
     </row>
     <row r="87">
       <c r="A87" t="n" s="10">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="B87" t="s" s="7">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="C87" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D87" t="s" s="7">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="E87" t="s" s="6">
         <v>2</v>
@@ -2004,16 +2010,16 @@
     </row>
     <row r="88">
       <c r="A88" t="n" s="10">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
       <c r="B88" t="s" s="7">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C88" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D88" t="s" s="7">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E88" t="s" s="6">
         <v>2</v>
@@ -2024,16 +2030,16 @@
     </row>
     <row r="89">
       <c r="A89" t="n" s="10">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
       <c r="B89" t="s" s="7">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C89" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D89" t="s" s="7">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E89" t="s" s="6">
         <v>2</v>
@@ -2044,16 +2050,16 @@
     </row>
     <row r="90">
       <c r="A90" t="n" s="10">
-        <v>7.0</v>
+        <v>5.0</v>
       </c>
       <c r="B90" t="s" s="7">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C90" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D90" t="s" s="7">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E90" t="s" s="6">
         <v>2</v>
@@ -2064,16 +2070,16 @@
     </row>
     <row r="91">
       <c r="A91" t="n" s="10">
-        <v>8.0</v>
+        <v>6.0</v>
       </c>
       <c r="B91" t="s" s="7">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C91" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D91" t="s" s="7">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E91" t="s" s="6">
         <v>2</v>
@@ -2084,16 +2090,16 @@
     </row>
     <row r="92">
       <c r="A92" t="n" s="10">
-        <v>9.0</v>
+        <v>7.0</v>
       </c>
       <c r="B92" t="s" s="7">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C92" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D92" t="s" s="7">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E92" t="s" s="6">
         <v>2</v>
@@ -2104,16 +2110,16 @@
     </row>
     <row r="93">
       <c r="A93" t="n" s="10">
-        <v>10.0</v>
+        <v>8.0</v>
       </c>
       <c r="B93" t="s" s="7">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C93" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D93" t="s" s="7">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E93" t="s" s="6">
         <v>2</v>
@@ -2124,16 +2130,16 @@
     </row>
     <row r="94">
       <c r="A94" t="n" s="10">
-        <v>11.0</v>
+        <v>9.0</v>
       </c>
       <c r="B94" t="s" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C94" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D94" t="s" s="7">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E94" t="s" s="6">
         <v>2</v>
@@ -2144,158 +2150,158 @@
     </row>
     <row r="95">
       <c r="A95" t="n" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="B95" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C95" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D95" t="s" s="7">
+        <v>47</v>
+      </c>
+      <c r="E95" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F95" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n" s="10">
+        <v>11.0</v>
+      </c>
+      <c r="B96" t="s" s="7">
+        <v>48</v>
+      </c>
+      <c r="C96" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D96" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="E96" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F96" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n" s="10">
         <v>12.0</v>
       </c>
-      <c r="B95" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="C95" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D95" t="s" s="7">
-        <v>72</v>
-      </c>
-      <c r="E95" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F95" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="96"/>
-    <row r="97"/>
-    <row r="98">
-      <c r="A98" t="s" s="4">
+      <c r="B97" t="s" s="7">
+        <v>50</v>
+      </c>
+      <c r="C97" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D97" t="s" s="7">
+        <v>74</v>
+      </c>
+      <c r="E97" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F97" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100">
+      <c r="A100" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B98" t="s" s="4">
-        <v>73</v>
-      </c>
-      <c r="C98" t="s" s="4">
+      <c r="B100" t="s" s="4">
+        <v>75</v>
+      </c>
+      <c r="C100" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D98" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E98" t="s" s="4">
+      <c r="D100" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E100" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F98" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="s" s="9">
+      <c r="F100" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B99" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C99" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D99" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E99" t="s" s="9">
+      <c r="B101" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C101" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D101" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E101" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F99" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s" s="8">
+      <c r="F101" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B100" t="s" s="8">
+      <c r="B102" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C100" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D100" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E100" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F100" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="s" s="5">
+      <c r="C102" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E102" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F102" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B101" t="s" s="5">
+      <c r="B103" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C101" t="s" s="5">
+      <c r="C103" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D101" t="s" s="5">
+      <c r="D103" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E101" t="s" s="5">
+      <c r="E103" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F101" t="s" s="5">
+      <c r="F103" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B102" t="s" s="7">
-        <v>56</v>
-      </c>
-      <c r="C102" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D102" t="s" s="7">
-        <v>57</v>
-      </c>
-      <c r="E102" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F102" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="n" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="B103" t="s" s="7">
-        <v>58</v>
-      </c>
-      <c r="C103" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D103" t="s" s="7">
-        <v>59</v>
-      </c>
-      <c r="E103" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F103" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n" s="10">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="B104" t="s" s="7">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="C104" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D104" t="s" s="7">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="E104" t="s" s="6">
         <v>2</v>
@@ -2306,16 +2312,16 @@
     </row>
     <row r="105">
       <c r="A105" t="n" s="10">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="B105" t="s" s="7">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="C105" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D105" t="s" s="7">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="E105" t="s" s="6">
         <v>2</v>
@@ -2324,138 +2330,100 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106">
-      <c r="A106" t="n" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="B106" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="C106" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D106" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="E106" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F106" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="n" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="B107" t="s" s="7">
-        <v>60</v>
-      </c>
-      <c r="C107" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D107" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="E107" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F107" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="106"/>
+    <row r="107"/>
     <row r="108">
-      <c r="A108" t="n" s="10">
-        <v>7.0</v>
-      </c>
-      <c r="B108" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="C108" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D108" t="s" s="7">
-        <v>41</v>
-      </c>
-      <c r="E108" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F108" t="s" s="6">
+      <c r="A108" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B108" t="s" s="4">
+        <v>77</v>
+      </c>
+      <c r="C108" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D108" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E108" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F108" t="s" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="n" s="10">
-        <v>8.0</v>
-      </c>
-      <c r="B109" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="C109" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D109" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="E109" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F109" t="s" s="6">
+      <c r="A109" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B109" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C109" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D109" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E109" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F109" t="s" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="n" s="10">
-        <v>9.0</v>
-      </c>
-      <c r="B110" t="s" s="7">
-        <v>44</v>
-      </c>
-      <c r="C110" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D110" t="s" s="7">
-        <v>45</v>
-      </c>
-      <c r="E110" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F110" t="s" s="6">
+      <c r="A110" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B110" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C110" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D110" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E110" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F110" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="n" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="B111" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C111" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D111" t="s" s="7">
-        <v>47</v>
-      </c>
-      <c r="E111" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F111" t="s" s="6">
-        <v>2</v>
+      <c r="A111" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B111" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C111" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D111" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E111" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F111" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n" s="10">
-        <v>11.0</v>
+        <v>1.0</v>
       </c>
       <c r="B112" t="s" s="7">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C112" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D112" t="s" s="7">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E112" t="s" s="6">
         <v>2</v>
@@ -2464,100 +2432,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="113"/>
-    <row r="114"/>
+    <row r="113">
+      <c r="A113" t="n" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="B113" t="s" s="7">
+        <v>59</v>
+      </c>
+      <c r="C113" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D113" t="s" s="7">
+        <v>60</v>
+      </c>
+      <c r="E113" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F113" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="B114" t="s" s="7">
+        <v>32</v>
+      </c>
+      <c r="C114" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D114" t="s" s="7">
+        <v>33</v>
+      </c>
+      <c r="E114" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F114" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="115">
-      <c r="A115" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B115" t="s" s="4">
-        <v>75</v>
-      </c>
-      <c r="C115" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D115" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E115" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F115" t="s" s="4">
+      <c r="A115" t="n" s="10">
+        <v>4.0</v>
+      </c>
+      <c r="B115" t="s" s="7">
+        <v>34</v>
+      </c>
+      <c r="C115" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D115" t="s" s="7">
+        <v>35</v>
+      </c>
+      <c r="E115" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F115" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B116" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C116" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D116" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E116" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F116" t="s" s="9">
+      <c r="A116" t="n" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="B116" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="C116" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D116" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="E116" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F116" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B117" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C117" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D117" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E117" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F117" t="s" s="8">
+      <c r="A117" t="n" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="B117" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="C117" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D117" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="E117" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F117" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B118" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C118" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D118" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E118" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F118" t="s" s="5">
-        <v>25</v>
+      <c r="A118" t="n" s="10">
+        <v>7.0</v>
+      </c>
+      <c r="B118" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="C118" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D118" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="E118" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F118" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n" s="10">
-        <v>1.0</v>
+        <v>8.0</v>
       </c>
       <c r="B119" t="s" s="7">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="C119" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D119" t="s" s="7">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="E119" t="s" s="6">
         <v>2</v>
@@ -2568,21 +2574,41 @@
     </row>
     <row r="120">
       <c r="A120" t="n" s="10">
-        <v>2.0</v>
+        <v>9.0</v>
       </c>
       <c r="B120" t="s" s="7">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="C120" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D120" t="s" s="7">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="E120" t="s" s="6">
         <v>2</v>
       </c>
       <c r="F120" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="B121" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C121" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D121" t="s" s="7">
+        <v>78</v>
+      </c>
+      <c r="E121" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F121" t="s" s="6">
         <v>2</v>
       </c>
     </row>
@@ -2596,14 +2622,14 @@
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B116:D116"/>
-    <mergeCell ref="B117:F117"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B84:F84"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B109:D109"/>
+    <mergeCell ref="B110:F110"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
From v1.2.1 to v1.2.3
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
+++ b/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
@@ -92,6 +92,126 @@
     <t>Actual Result</t>
   </si>
   <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de viagem nacional - fora do estado (interestadual).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: viagem nacional - fora do estado (interestadual).</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o estado.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: estado.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe a(s) cidade(s).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: cidade(s).</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de deslocamento.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: tipo de deslocamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de hospedagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: hospedagem.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Escolhe o tipo de periodo de afastamento.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: periodo de afastamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa as datas de afastamento, apos o ultimo dia de viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: pernoite.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Detalha a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe os beneficiarios selecionados e o campo para preenchimento do nome social</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa o nome social do beneficiario da(s) diaria(s)</t>
+  </si>
+  <si>
+    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Clica em confirmar.</t>
+  </si>
+  <si>
+    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado. 3. Manutenção do cargo comissionado e do setor beneficiário à época da concessão da diária.</t>
+  </si>
+  <si>
+    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>O sistema salva os dados</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa as datas de afastamento, antes do ultimo dia de viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe os beneficiarios selecionados.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Clica em limpar campos.</t>
+  </si>
+  <si>
+    <t>SYSTEM Apaga todas as seleções do usuário.</t>
+  </si>
+  <si>
+    <t>TC3</t>
+  </si>
+  <si>
     <t>Chefe/Beneficiário Seleciona o tipo de viagem nacional - dentro do estado (intermunicipal).</t>
   </si>
   <si>
@@ -104,151 +224,31 @@
     <t>SYSTEM O sistema seleciona o estado como PB, automaticamente.</t>
   </si>
   <si>
-    <t>Chefe/Beneficiário Escolhe a(s) cidade(s).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: cidade(s).</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de deslocamento.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: tipo de deslocamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de hospedagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: hospedagem.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de periodo de afastamento.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: periodo de afastamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa as datas de afastamento, antes do ultimo dia de viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: pernoite.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Detalha a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe os beneficiarios selecionados e o campo para preenchimento do nome social</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa o nome social do beneficiario da(s) diaria(s)</t>
-  </si>
-  <si>
-    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Clica em confirmar.</t>
-  </si>
-  <si>
-    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado. 3. Manutenção do cargo comissionado e do setor beneficiário à época da concessão da diária.</t>
-  </si>
-  <si>
-    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>O sistema salva os dados</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa as datas de afastamento, apos o ultimo dia de viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe os beneficiarios selecionados.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Clica em limpar campos.</t>
-  </si>
-  <si>
-    <t>SYSTEM Apaga todas as seleções do usuário.</t>
-  </si>
-  <si>
-    <t>TC3</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o tipo de viagem nacional - fora do estado (interestadual).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: viagem nacional - fora do estado (interestadual).</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Escolhe o estado.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: estado.</t>
+    <t>SYSTEM Não confirma a existencia de conta para recebimento de diarias do servidor. Exibe a mensagem de erro MSG002 - Conta para recebimento de diárias não cadastrada.</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
+  </si>
+  <si>
+    <t>TC5</t>
   </si>
   <si>
     <t>SYSTEM Exibe a mensagem de erro MSG202 - RGP Core indisponível.</t>
   </si>
   <si>
-    <t>TC4</t>
+    <t>TC6</t>
   </si>
   <si>
     <t>SYSTEM Exibe a mensagem de erro MSG203 - Campos obrigatórios, MSG214 - Campos obrigatórios da solicitação de diárias (não informados).</t>
   </si>
   <si>
-    <t>TC5</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
-  </si>
-  <si>
-    <t>TC6</t>
+    <t>TC7</t>
   </si>
   <si>
     <t>SYSTEM Exibe a mensagem de erro MSG201 - DNE indisponível.</t>
-  </si>
-  <si>
-    <t>TC7</t>
-  </si>
-  <si>
-    <t>SYSTEM Não confirma a existencia de conta para recebimento de diarias do servidor. Exibe a mensagem de erro MSG002 - Conta para recebimento de diárias não cadastrada.</t>
   </si>
 </sst>
 </file>
@@ -1515,7 +1515,7 @@
         <v>2</v>
       </c>
       <c r="D59" t="s" s="7">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="E59" t="s" s="6">
         <v>2</v>
@@ -1524,120 +1524,120 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60">
-      <c r="A60" t="n" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B60" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C60" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D60" t="s" s="7">
-        <v>70</v>
-      </c>
-      <c r="E60" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F60" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="60"/>
     <row r="61"/>
-    <row r="62"/>
+    <row r="62">
+      <c r="A62" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B62" t="s" s="4">
+        <v>71</v>
+      </c>
+      <c r="C62" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D62" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E62" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F62" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
     <row r="63">
-      <c r="A63" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B63" t="s" s="4">
-        <v>71</v>
-      </c>
-      <c r="C63" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D63" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E63" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F63" t="s" s="4">
+      <c r="A63" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B63" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C63" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D63" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E63" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F63" t="s" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D64" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E64" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F64" t="s" s="9">
+      <c r="A64" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B64" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C64" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F64" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B65" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E65" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F65" t="s" s="8">
-        <v>2</v>
+      <c r="A65" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B65" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C65" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D65" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E65" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F65" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B66" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C66" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D66" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E66" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F66" t="s" s="5">
-        <v>25</v>
+      <c r="A66" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B66" t="s" s="7">
+        <v>57</v>
+      </c>
+      <c r="C66" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D66" t="s" s="7">
+        <v>58</v>
+      </c>
+      <c r="E66" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F66" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n" s="10">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B67" t="s" s="7">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C67" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D67" t="s" s="7">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="E67" t="s" s="6">
         <v>2</v>
@@ -1648,16 +1648,16 @@
     </row>
     <row r="68">
       <c r="A68" t="n" s="10">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="B68" t="s" s="7">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="C68" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D68" t="s" s="7">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="E68" t="s" s="6">
         <v>2</v>
@@ -1668,16 +1668,16 @@
     </row>
     <row r="69">
       <c r="A69" t="n" s="10">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="B69" t="s" s="7">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C69" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D69" t="s" s="7">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E69" t="s" s="6">
         <v>2</v>
@@ -1688,16 +1688,16 @@
     </row>
     <row r="70">
       <c r="A70" t="n" s="10">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="B70" t="s" s="7">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C70" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D70" t="s" s="7">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E70" t="s" s="6">
         <v>2</v>
@@ -1708,16 +1708,16 @@
     </row>
     <row r="71">
       <c r="A71" t="n" s="10">
-        <v>5.0</v>
+        <v>6.0</v>
       </c>
       <c r="B71" t="s" s="7">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C71" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D71" t="s" s="7">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E71" t="s" s="6">
         <v>2</v>
@@ -1728,16 +1728,16 @@
     </row>
     <row r="72">
       <c r="A72" t="n" s="10">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="B72" t="s" s="7">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C72" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D72" t="s" s="7">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="E72" t="s" s="6">
         <v>2</v>
@@ -1748,16 +1748,16 @@
     </row>
     <row r="73">
       <c r="A73" t="n" s="10">
-        <v>7.0</v>
+        <v>8.0</v>
       </c>
       <c r="B73" t="s" s="7">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="C73" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D73" t="s" s="7">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E73" t="s" s="6">
         <v>2</v>
@@ -1768,16 +1768,16 @@
     </row>
     <row r="74">
       <c r="A74" t="n" s="10">
-        <v>8.0</v>
+        <v>9.0</v>
       </c>
       <c r="B74" t="s" s="7">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C74" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D74" t="s" s="7">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E74" t="s" s="6">
         <v>2</v>
@@ -1788,16 +1788,16 @@
     </row>
     <row r="75">
       <c r="A75" t="n" s="10">
-        <v>9.0</v>
+        <v>10.0</v>
       </c>
       <c r="B75" t="s" s="7">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C75" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D75" t="s" s="7">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E75" t="s" s="6">
         <v>2</v>
@@ -1808,16 +1808,16 @@
     </row>
     <row r="76">
       <c r="A76" t="n" s="10">
-        <v>10.0</v>
+        <v>11.0</v>
       </c>
       <c r="B76" t="s" s="7">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C76" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D76" t="s" s="7">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E76" t="s" s="6">
         <v>2</v>
@@ -1828,16 +1828,16 @@
     </row>
     <row r="77">
       <c r="A77" t="n" s="10">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
       <c r="B77" t="s" s="7">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C77" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D77" t="s" s="7">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E77" t="s" s="6">
         <v>2</v>
@@ -1846,140 +1846,140 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" t="n" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B78" t="s" s="7">
-        <v>46</v>
-      </c>
-      <c r="C78" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D78" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="E78" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F78" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="n" s="10">
-        <v>13.0</v>
-      </c>
-      <c r="B79" t="s" s="7">
-        <v>50</v>
-      </c>
-      <c r="C79" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D79" t="s" s="7">
-        <v>72</v>
-      </c>
-      <c r="E79" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F79" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80"/>
-    <row r="81"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80">
+      <c r="A80" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B80" t="s" s="4">
+        <v>73</v>
+      </c>
+      <c r="C80" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D80" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E80" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F80" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B81" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E81" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F81" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
     <row r="82">
-      <c r="A82" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B82" t="s" s="4">
-        <v>73</v>
-      </c>
-      <c r="C82" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D82" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E82" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F82" t="s" s="4">
+      <c r="A82" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B82" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C82" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E82" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F82" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B83" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C83" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D83" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E83" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F83" t="s" s="9">
-        <v>2</v>
+      <c r="A83" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B83" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C83" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D83" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E83" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F83" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B84" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C84" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D84" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E84" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F84" t="s" s="8">
+      <c r="A84" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B84" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="C84" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D84" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="E84" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F84" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B85" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C85" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D85" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E85" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F85" t="s" s="5">
-        <v>25</v>
+      <c r="A85" t="n" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="B85" t="s" s="7">
+        <v>28</v>
+      </c>
+      <c r="C85" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D85" t="s" s="7">
+        <v>29</v>
+      </c>
+      <c r="E85" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F85" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n" s="10">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B86" t="s" s="7">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="C86" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D86" t="s" s="7">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="E86" t="s" s="6">
         <v>2</v>
@@ -1990,16 +1990,16 @@
     </row>
     <row r="87">
       <c r="A87" t="n" s="10">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B87" t="s" s="7">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="C87" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D87" t="s" s="7">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="E87" t="s" s="6">
         <v>2</v>
@@ -2010,16 +2010,16 @@
     </row>
     <row r="88">
       <c r="A88" t="n" s="10">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="B88" t="s" s="7">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C88" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D88" t="s" s="7">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E88" t="s" s="6">
         <v>2</v>
@@ -2030,16 +2030,16 @@
     </row>
     <row r="89">
       <c r="A89" t="n" s="10">
-        <v>4.0</v>
+        <v>6.0</v>
       </c>
       <c r="B89" t="s" s="7">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C89" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D89" t="s" s="7">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E89" t="s" s="6">
         <v>2</v>
@@ -2050,16 +2050,16 @@
     </row>
     <row r="90">
       <c r="A90" t="n" s="10">
-        <v>5.0</v>
+        <v>7.0</v>
       </c>
       <c r="B90" t="s" s="7">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C90" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D90" t="s" s="7">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E90" t="s" s="6">
         <v>2</v>
@@ -2070,16 +2070,16 @@
     </row>
     <row r="91">
       <c r="A91" t="n" s="10">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
       <c r="B91" t="s" s="7">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C91" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D91" t="s" s="7">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E91" t="s" s="6">
         <v>2</v>
@@ -2090,16 +2090,16 @@
     </row>
     <row r="92">
       <c r="A92" t="n" s="10">
-        <v>7.0</v>
+        <v>9.0</v>
       </c>
       <c r="B92" t="s" s="7">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C92" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D92" t="s" s="7">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E92" t="s" s="6">
         <v>2</v>
@@ -2110,16 +2110,16 @@
     </row>
     <row r="93">
       <c r="A93" t="n" s="10">
-        <v>8.0</v>
+        <v>10.0</v>
       </c>
       <c r="B93" t="s" s="7">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C93" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D93" t="s" s="7">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E93" t="s" s="6">
         <v>2</v>
@@ -2130,16 +2130,16 @@
     </row>
     <row r="94">
       <c r="A94" t="n" s="10">
-        <v>9.0</v>
+        <v>11.0</v>
       </c>
       <c r="B94" t="s" s="7">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C94" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D94" t="s" s="7">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E94" t="s" s="6">
         <v>2</v>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="95">
       <c r="A95" t="n" s="10">
-        <v>10.0</v>
+        <v>12.0</v>
       </c>
       <c r="B95" t="s" s="7">
         <v>46</v>
@@ -2159,7 +2159,7 @@
         <v>2</v>
       </c>
       <c r="D95" t="s" s="7">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="E95" t="s" s="6">
         <v>2</v>
@@ -2168,140 +2168,140 @@
         <v>2</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" t="n" s="10">
-        <v>11.0</v>
-      </c>
-      <c r="B96" t="s" s="7">
-        <v>48</v>
-      </c>
-      <c r="C96" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D96" t="s" s="7">
-        <v>49</v>
-      </c>
-      <c r="E96" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F96" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="n" s="10">
-        <v>12.0</v>
-      </c>
-      <c r="B97" t="s" s="7">
-        <v>50</v>
-      </c>
-      <c r="C97" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D97" t="s" s="7">
-        <v>74</v>
-      </c>
-      <c r="E97" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F97" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="98"/>
-    <row r="99"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98">
+      <c r="A98" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B98" t="s" s="4">
+        <v>75</v>
+      </c>
+      <c r="C98" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D98" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E98" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F98" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B99" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C99" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D99" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E99" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F99" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
     <row r="100">
-      <c r="A100" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B100" t="s" s="4">
-        <v>75</v>
-      </c>
-      <c r="C100" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D100" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E100" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F100" t="s" s="4">
+      <c r="A100" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B100" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C100" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D100" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E100" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F100" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B101" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C101" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D101" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E101" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F101" t="s" s="9">
-        <v>2</v>
+      <c r="A101" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B101" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C101" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D101" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E101" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F101" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B102" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C102" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D102" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E102" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F102" t="s" s="8">
+      <c r="A102" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B102" t="s" s="7">
+        <v>57</v>
+      </c>
+      <c r="C102" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D102" t="s" s="7">
+        <v>58</v>
+      </c>
+      <c r="E102" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F102" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B103" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C103" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D103" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E103" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F103" t="s" s="5">
-        <v>25</v>
+      <c r="A103" t="n" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="B103" t="s" s="7">
+        <v>59</v>
+      </c>
+      <c r="C103" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D103" t="s" s="7">
+        <v>60</v>
+      </c>
+      <c r="E103" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F103" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n" s="10">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B104" t="s" s="7">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="C104" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D104" t="s" s="7">
-        <v>67</v>
+        <v>33</v>
       </c>
       <c r="E104" t="s" s="6">
         <v>2</v>
@@ -2312,16 +2312,16 @@
     </row>
     <row r="105">
       <c r="A105" t="n" s="10">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="B105" t="s" s="7">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="C105" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D105" t="s" s="7">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="E105" t="s" s="6">
         <v>2</v>
@@ -2330,100 +2330,138 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106"/>
-    <row r="107"/>
+    <row r="106">
+      <c r="A106" t="n" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="B106" t="s" s="7">
+        <v>36</v>
+      </c>
+      <c r="C106" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D106" t="s" s="7">
+        <v>37</v>
+      </c>
+      <c r="E106" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F106" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n" s="10">
+        <v>6.0</v>
+      </c>
+      <c r="B107" t="s" s="7">
+        <v>38</v>
+      </c>
+      <c r="C107" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D107" t="s" s="7">
+        <v>39</v>
+      </c>
+      <c r="E107" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F107" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="108">
-      <c r="A108" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="B108" t="s" s="4">
-        <v>77</v>
-      </c>
-      <c r="C108" t="s" s="4">
-        <v>14</v>
-      </c>
-      <c r="D108" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E108" t="s" s="4">
-        <v>15</v>
-      </c>
-      <c r="F108" t="s" s="4">
+      <c r="A108" t="n" s="10">
+        <v>7.0</v>
+      </c>
+      <c r="B108" t="s" s="7">
+        <v>40</v>
+      </c>
+      <c r="C108" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D108" t="s" s="7">
+        <v>41</v>
+      </c>
+      <c r="E108" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F108" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="B109" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C109" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D109" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E109" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="F109" t="s" s="9">
+      <c r="A109" t="n" s="10">
+        <v>8.0</v>
+      </c>
+      <c r="B109" t="s" s="7">
+        <v>42</v>
+      </c>
+      <c r="C109" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D109" t="s" s="7">
+        <v>43</v>
+      </c>
+      <c r="E109" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F109" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="s" s="8">
-        <v>18</v>
-      </c>
-      <c r="B110" t="s" s="8">
-        <v>19</v>
-      </c>
-      <c r="C110" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D110" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E110" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F110" t="s" s="8">
+      <c r="A110" t="n" s="10">
+        <v>9.0</v>
+      </c>
+      <c r="B110" t="s" s="7">
+        <v>44</v>
+      </c>
+      <c r="C110" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D110" t="s" s="7">
+        <v>45</v>
+      </c>
+      <c r="E110" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F110" t="s" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="B111" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="C111" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="D111" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="E111" t="s" s="5">
-        <v>24</v>
-      </c>
-      <c r="F111" t="s" s="5">
-        <v>25</v>
+      <c r="A111" t="n" s="10">
+        <v>10.0</v>
+      </c>
+      <c r="B111" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C111" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D111" t="s" s="7">
+        <v>62</v>
+      </c>
+      <c r="E111" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F111" t="s" s="6">
+        <v>2</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n" s="10">
-        <v>1.0</v>
+        <v>11.0</v>
       </c>
       <c r="B112" t="s" s="7">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C112" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D112" t="s" s="7">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E112" t="s" s="6">
         <v>2</v>
@@ -2434,16 +2472,16 @@
     </row>
     <row r="113">
       <c r="A113" t="n" s="10">
-        <v>2.0</v>
+        <v>12.0</v>
       </c>
       <c r="B113" t="s" s="7">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C113" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D113" t="s" s="7">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="E113" t="s" s="6">
         <v>2</v>
@@ -2452,138 +2490,100 @@
         <v>2</v>
       </c>
     </row>
-    <row r="114">
-      <c r="A114" t="n" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="B114" t="s" s="7">
-        <v>32</v>
-      </c>
-      <c r="C114" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D114" t="s" s="7">
-        <v>33</v>
-      </c>
-      <c r="E114" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F114" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="n" s="10">
-        <v>4.0</v>
-      </c>
-      <c r="B115" t="s" s="7">
-        <v>34</v>
-      </c>
-      <c r="C115" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D115" t="s" s="7">
-        <v>35</v>
-      </c>
-      <c r="E115" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F115" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
+    <row r="114"/>
+    <row r="115"/>
     <row r="116">
-      <c r="A116" t="n" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="B116" t="s" s="7">
-        <v>36</v>
-      </c>
-      <c r="C116" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D116" t="s" s="7">
-        <v>37</v>
-      </c>
-      <c r="E116" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F116" t="s" s="6">
+      <c r="A116" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="B116" t="s" s="4">
+        <v>77</v>
+      </c>
+      <c r="C116" t="s" s="4">
+        <v>14</v>
+      </c>
+      <c r="D116" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E116" t="s" s="4">
+        <v>15</v>
+      </c>
+      <c r="F116" t="s" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="n" s="10">
-        <v>6.0</v>
-      </c>
-      <c r="B117" t="s" s="7">
-        <v>38</v>
-      </c>
-      <c r="C117" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D117" t="s" s="7">
-        <v>39</v>
-      </c>
-      <c r="E117" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F117" t="s" s="6">
+      <c r="A117" t="s" s="9">
+        <v>16</v>
+      </c>
+      <c r="B117" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C117" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D117" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E117" t="s" s="9">
+        <v>17</v>
+      </c>
+      <c r="F117" t="s" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="n" s="10">
-        <v>7.0</v>
-      </c>
-      <c r="B118" t="s" s="7">
-        <v>40</v>
-      </c>
-      <c r="C118" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D118" t="s" s="7">
-        <v>41</v>
-      </c>
-      <c r="E118" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F118" t="s" s="6">
+      <c r="A118" t="s" s="8">
+        <v>18</v>
+      </c>
+      <c r="B118" t="s" s="8">
+        <v>19</v>
+      </c>
+      <c r="C118" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D118" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E118" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F118" t="s" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="n" s="10">
-        <v>8.0</v>
-      </c>
-      <c r="B119" t="s" s="7">
-        <v>42</v>
-      </c>
-      <c r="C119" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D119" t="s" s="7">
-        <v>43</v>
-      </c>
-      <c r="E119" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F119" t="s" s="6">
-        <v>2</v>
+      <c r="A119" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B119" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C119" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D119" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="E119" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="F119" t="s" s="5">
+        <v>25</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n" s="10">
-        <v>9.0</v>
+        <v>1.0</v>
       </c>
       <c r="B120" t="s" s="7">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C120" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D120" t="s" s="7">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="E120" t="s" s="6">
         <v>2</v>
@@ -2594,10 +2594,10 @@
     </row>
     <row r="121">
       <c r="A121" t="n" s="10">
-        <v>10.0</v>
+        <v>2.0</v>
       </c>
       <c r="B121" t="s" s="7">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="C121" t="s" s="6">
         <v>2</v>
@@ -2622,14 +2622,14 @@
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B65:F65"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B84:F84"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B109:D109"/>
-    <mergeCell ref="B110:F110"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B64:F64"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="B100:F100"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="B118:F118"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
From v1.2.3 to v1.2.4
</commit_message>
<xml_diff>
--- a/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
+++ b/output/xlsx/UC001 - Solicitar diarias--GT-.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="79">
   <si>
     <t xml:space="preserve">System: </t>
   </si>
@@ -128,78 +128,78 @@
     <t>SYSTEM Exibe a opcao escolhida: periodo de afastamento.</t>
   </si>
   <si>
+    <t>Chefe/Beneficiário Informa as datas de afastamento, antes do ultimo dia de viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: pernoite.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Detalha a justificativa.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe os beneficiarios selecionados e o campo para preenchimento do nome social</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Informa o nome social do beneficiario da(s) diaria(s)</t>
+  </si>
+  <si>
+    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Clica em confirmar.</t>
+  </si>
+  <si>
+    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado. 3. Manutenção do cargo comissionado e do setor beneficiário à época da concessão da diária.</t>
+  </si>
+  <si>
+    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcondition: </t>
+  </si>
+  <si>
+    <t>O sistema salva os dados</t>
+  </si>
+  <si>
+    <t>TC2</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
+  </si>
+  <si>
+    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
+  </si>
+  <si>
     <t>Chefe/Beneficiário Informa as datas de afastamento, apos o ultimo dia de viagem.</t>
   </si>
   <si>
-    <t>SYSTEM Exibe as datas escolhidas: datas de afastamento.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa se tem pernoite.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: pernoite.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Detalha a justificativa.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe o texto informado: detalhe da justificativa.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o(s) beneficiarios da(s) diaria(s).</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe os beneficiarios selecionados e o campo para preenchimento do nome social</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa o nome social do beneficiario da(s) diaria(s)</t>
-  </si>
-  <si>
-    <t>SYSTEM Confirma a existencia de conta para recebimento de diarias do servidor.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Clica em confirmar.</t>
-  </si>
-  <si>
-    <t>SYSTEM Calcula o valor da(s) diaria(s) com as informacoes do formulario.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Verifica os valores presentes na tela: 1. Magistrados e desembargadores: não podem ultrapassar 60% do valor de um diária de um ministro do STF. 2. Servidores não podem ultrapassar 60% do valor de uma diária de um Magistrado. 3. Manutenção do cargo comissionado e do setor beneficiário à época da concessão da diária.</t>
-  </si>
-  <si>
-    <t>SYSTEM Altera o status da diaria para SOLICITADA: (antes) para empenho; ou, (depois) para prestação de contas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postcondition: </t>
-  </si>
-  <si>
-    <t>O sistema salva os dados</t>
-  </si>
-  <si>
-    <t>TC2</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o tipo de viagem internacional.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a lista de países para seleção, no lugar de estado/cidade.</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Seleciona o país da viagem.</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a opcao escolhida: país da viagem</t>
-  </si>
-  <si>
-    <t>Chefe/Beneficiário Informa as datas de afastamento, antes do ultimo dia de viagem.</t>
-  </si>
-  <si>
     <t>SYSTEM Exibe os beneficiarios selecionados.</t>
   </si>
   <si>
@@ -224,19 +224,19 @@
     <t>SYSTEM O sistema seleciona o estado como PB, automaticamente.</t>
   </si>
   <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG202 - RGP Core indisponível.</t>
+  </si>
+  <si>
+    <t>TC4</t>
+  </si>
+  <si>
+    <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
     <t>SYSTEM Não confirma a existencia de conta para recebimento de diarias do servidor. Exibe a mensagem de erro MSG002 - Conta para recebimento de diárias não cadastrada.</t>
-  </si>
-  <si>
-    <t>TC4</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG204 - Conflito de duplicidade de diárias.</t>
-  </si>
-  <si>
-    <t>TC5</t>
-  </si>
-  <si>
-    <t>SYSTEM Exibe a mensagem de erro MSG202 - RGP Core indisponível.</t>
   </si>
   <si>
     <t>TC6</t>
@@ -444,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F122"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="false"/>
   </sheetViews>
@@ -1429,7 +1429,7 @@
         <v>7.0</v>
       </c>
       <c r="B55" t="s" s="7">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="C55" t="s" s="6">
         <v>2</v>
@@ -1515,129 +1515,129 @@
         <v>2</v>
       </c>
       <c r="D59" t="s" s="7">
+        <v>62</v>
+      </c>
+      <c r="E59" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F59" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n" s="10">
+        <v>12.0</v>
+      </c>
+      <c r="B60" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C60" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D60" t="s" s="7">
         <v>70</v>
       </c>
-      <c r="E59" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F59" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60"/>
+      <c r="E60" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F60" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="61"/>
-    <row r="62">
-      <c r="A62" t="s" s="4">
+    <row r="62"/>
+    <row r="63">
+      <c r="A63" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B62" t="s" s="4">
+      <c r="B63" t="s" s="4">
         <v>71</v>
       </c>
-      <c r="C62" t="s" s="4">
+      <c r="C63" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D62" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E62" t="s" s="4">
+      <c r="D63" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E63" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F62" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s" s="9">
+      <c r="F63" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B63" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C63" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D63" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E63" t="s" s="9">
+      <c r="B64" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D64" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E64" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F63" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s" s="8">
+      <c r="F64" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B64" t="s" s="8">
+      <c r="B65" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C64" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D64" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E64" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F64" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s" s="5">
+      <c r="C65" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D65" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F65" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B65" t="s" s="5">
+      <c r="B66" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C65" t="s" s="5">
+      <c r="C66" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D65" t="s" s="5">
+      <c r="D66" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E65" t="s" s="5">
+      <c r="E66" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F65" t="s" s="5">
+      <c r="F66" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B66" t="s" s="7">
-        <v>57</v>
-      </c>
-      <c r="C66" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D66" t="s" s="7">
-        <v>58</v>
-      </c>
-      <c r="E66" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F66" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n" s="10">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B67" t="s" s="7">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C67" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D67" t="s" s="7">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E67" t="s" s="6">
         <v>2</v>
@@ -1648,16 +1648,16 @@
     </row>
     <row r="68">
       <c r="A68" t="n" s="10">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B68" t="s" s="7">
-        <v>32</v>
+        <v>59</v>
       </c>
       <c r="C68" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D68" t="s" s="7">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="E68" t="s" s="6">
         <v>2</v>
@@ -1668,16 +1668,16 @@
     </row>
     <row r="69">
       <c r="A69" t="n" s="10">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B69" t="s" s="7">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C69" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D69" t="s" s="7">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E69" t="s" s="6">
         <v>2</v>
@@ -1688,16 +1688,16 @@
     </row>
     <row r="70">
       <c r="A70" t="n" s="10">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B70" t="s" s="7">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C70" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D70" t="s" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E70" t="s" s="6">
         <v>2</v>
@@ -1708,16 +1708,16 @@
     </row>
     <row r="71">
       <c r="A71" t="n" s="10">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B71" t="s" s="7">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C71" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D71" t="s" s="7">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E71" t="s" s="6">
         <v>2</v>
@@ -1728,16 +1728,16 @@
     </row>
     <row r="72">
       <c r="A72" t="n" s="10">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B72" t="s" s="7">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C72" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D72" t="s" s="7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E72" t="s" s="6">
         <v>2</v>
@@ -1748,16 +1748,16 @@
     </row>
     <row r="73">
       <c r="A73" t="n" s="10">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B73" t="s" s="7">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C73" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D73" t="s" s="7">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E73" t="s" s="6">
         <v>2</v>
@@ -1768,16 +1768,16 @@
     </row>
     <row r="74">
       <c r="A74" t="n" s="10">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B74" t="s" s="7">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C74" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D74" t="s" s="7">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E74" t="s" s="6">
         <v>2</v>
@@ -1788,16 +1788,16 @@
     </row>
     <row r="75">
       <c r="A75" t="n" s="10">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="B75" t="s" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C75" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D75" t="s" s="7">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E75" t="s" s="6">
         <v>2</v>
@@ -1808,16 +1808,16 @@
     </row>
     <row r="76">
       <c r="A76" t="n" s="10">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="B76" t="s" s="7">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C76" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D76" t="s" s="7">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E76" t="s" s="6">
         <v>2</v>
@@ -1828,138 +1828,138 @@
     </row>
     <row r="77">
       <c r="A77" t="n" s="10">
+        <v>11.0</v>
+      </c>
+      <c r="B77" t="s" s="7">
+        <v>48</v>
+      </c>
+      <c r="C77" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D77" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="E77" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F77" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n" s="10">
         <v>12.0</v>
       </c>
-      <c r="B77" t="s" s="7">
+      <c r="B78" t="s" s="7">
         <v>50</v>
       </c>
-      <c r="C77" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D77" t="s" s="7">
+      <c r="C78" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s" s="7">
         <v>72</v>
       </c>
-      <c r="E77" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F77" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="78"/>
+      <c r="E78" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F78" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="79"/>
-    <row r="80">
-      <c r="A80" t="s" s="4">
+    <row r="80"/>
+    <row r="81">
+      <c r="A81" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B80" t="s" s="4">
+      <c r="B81" t="s" s="4">
         <v>73</v>
       </c>
-      <c r="C80" t="s" s="4">
+      <c r="C81" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D80" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E80" t="s" s="4">
+      <c r="D81" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E81" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F80" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s" s="9">
+      <c r="F81" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B81" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C81" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D81" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E81" t="s" s="9">
+      <c r="B82" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C82" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D82" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E82" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F81" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s" s="8">
+      <c r="F82" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B82" t="s" s="8">
+      <c r="B83" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C82" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D82" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E82" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F82" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s" s="5">
+      <c r="C83" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D83" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E83" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F83" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B83" t="s" s="5">
+      <c r="B84" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C83" t="s" s="5">
+      <c r="C84" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D83" t="s" s="5">
+      <c r="D84" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E83" t="s" s="5">
+      <c r="E84" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F83" t="s" s="5">
+      <c r="F84" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B84" t="s" s="7">
-        <v>26</v>
-      </c>
-      <c r="C84" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D84" t="s" s="7">
-        <v>27</v>
-      </c>
-      <c r="E84" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F84" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n" s="10">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B85" t="s" s="7">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="C85" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D85" t="s" s="7">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="E85" t="s" s="6">
         <v>2</v>
@@ -1970,16 +1970,16 @@
     </row>
     <row r="86">
       <c r="A86" t="n" s="10">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B86" t="s" s="7">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="C86" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D86" t="s" s="7">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="E86" t="s" s="6">
         <v>2</v>
@@ -1990,16 +1990,16 @@
     </row>
     <row r="87">
       <c r="A87" t="n" s="10">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B87" t="s" s="7">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C87" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D87" t="s" s="7">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E87" t="s" s="6">
         <v>2</v>
@@ -2010,16 +2010,16 @@
     </row>
     <row r="88">
       <c r="A88" t="n" s="10">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B88" t="s" s="7">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C88" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D88" t="s" s="7">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E88" t="s" s="6">
         <v>2</v>
@@ -2030,16 +2030,16 @@
     </row>
     <row r="89">
       <c r="A89" t="n" s="10">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B89" t="s" s="7">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C89" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D89" t="s" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E89" t="s" s="6">
         <v>2</v>
@@ -2050,16 +2050,16 @@
     </row>
     <row r="90">
       <c r="A90" t="n" s="10">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B90" t="s" s="7">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C90" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D90" t="s" s="7">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E90" t="s" s="6">
         <v>2</v>
@@ -2070,16 +2070,16 @@
     </row>
     <row r="91">
       <c r="A91" t="n" s="10">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B91" t="s" s="7">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="C91" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D91" t="s" s="7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E91" t="s" s="6">
         <v>2</v>
@@ -2090,16 +2090,16 @@
     </row>
     <row r="92">
       <c r="A92" t="n" s="10">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B92" t="s" s="7">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C92" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D92" t="s" s="7">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E92" t="s" s="6">
         <v>2</v>
@@ -2110,16 +2110,16 @@
     </row>
     <row r="93">
       <c r="A93" t="n" s="10">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="B93" t="s" s="7">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C93" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D93" t="s" s="7">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E93" t="s" s="6">
         <v>2</v>
@@ -2130,16 +2130,16 @@
     </row>
     <row r="94">
       <c r="A94" t="n" s="10">
-        <v>11.0</v>
+        <v>10.0</v>
       </c>
       <c r="B94" t="s" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C94" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D94" t="s" s="7">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E94" t="s" s="6">
         <v>2</v>
@@ -2150,7 +2150,7 @@
     </row>
     <row r="95">
       <c r="A95" t="n" s="10">
-        <v>12.0</v>
+        <v>11.0</v>
       </c>
       <c r="B95" t="s" s="7">
         <v>46</v>
@@ -2255,13 +2255,13 @@
         <v>1.0</v>
       </c>
       <c r="B102" t="s" s="7">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C102" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D102" t="s" s="7">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E102" t="s" s="6">
         <v>2</v>
@@ -2275,13 +2275,13 @@
         <v>2.0</v>
       </c>
       <c r="B103" t="s" s="7">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C103" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D103" t="s" s="7">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="E103" t="s" s="6">
         <v>2</v>
@@ -2295,13 +2295,13 @@
         <v>3.0</v>
       </c>
       <c r="B104" t="s" s="7">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C104" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D104" t="s" s="7">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E104" t="s" s="6">
         <v>2</v>
@@ -2315,13 +2315,13 @@
         <v>4.0</v>
       </c>
       <c r="B105" t="s" s="7">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C105" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D105" t="s" s="7">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E105" t="s" s="6">
         <v>2</v>
@@ -2335,13 +2335,13 @@
         <v>5.0</v>
       </c>
       <c r="B106" t="s" s="7">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C106" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D106" t="s" s="7">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E106" t="s" s="6">
         <v>2</v>
@@ -2355,13 +2355,13 @@
         <v>6.0</v>
       </c>
       <c r="B107" t="s" s="7">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C107" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D107" t="s" s="7">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E107" t="s" s="6">
         <v>2</v>
@@ -2375,13 +2375,13 @@
         <v>7.0</v>
       </c>
       <c r="B108" t="s" s="7">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C108" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D108" t="s" s="7">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E108" t="s" s="6">
         <v>2</v>
@@ -2395,13 +2395,13 @@
         <v>8.0</v>
       </c>
       <c r="B109" t="s" s="7">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C109" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D109" t="s" s="7">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E109" t="s" s="6">
         <v>2</v>
@@ -2415,13 +2415,13 @@
         <v>9.0</v>
       </c>
       <c r="B110" t="s" s="7">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C110" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D110" t="s" s="7">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E110" t="s" s="6">
         <v>2</v>
@@ -2435,13 +2435,13 @@
         <v>10.0</v>
       </c>
       <c r="B111" t="s" s="7">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C111" t="s" s="6">
         <v>2</v>
       </c>
       <c r="D111" t="s" s="7">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E111" t="s" s="6">
         <v>2</v>
@@ -2461,7 +2461,7 @@
         <v>2</v>
       </c>
       <c r="D112" t="s" s="7">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E112" t="s" s="6">
         <v>2</v>
@@ -2475,140 +2475,160 @@
         <v>12.0</v>
       </c>
       <c r="B113" t="s" s="7">
+        <v>46</v>
+      </c>
+      <c r="C113" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D113" t="s" s="7">
+        <v>49</v>
+      </c>
+      <c r="E113" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F113" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n" s="10">
+        <v>13.0</v>
+      </c>
+      <c r="B114" t="s" s="7">
         <v>50</v>
       </c>
-      <c r="C113" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D113" t="s" s="7">
+      <c r="C114" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D114" t="s" s="7">
         <v>76</v>
       </c>
-      <c r="E113" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F113" t="s" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="114"/>
+      <c r="E114" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F114" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="115"/>
-    <row r="116">
-      <c r="A116" t="s" s="4">
+    <row r="116"/>
+    <row r="117">
+      <c r="A117" t="s" s="4">
         <v>12</v>
       </c>
-      <c r="B116" t="s" s="4">
+      <c r="B117" t="s" s="4">
         <v>77</v>
       </c>
-      <c r="C116" t="s" s="4">
+      <c r="C117" t="s" s="4">
         <v>14</v>
       </c>
-      <c r="D116" t="s" s="4">
-        <v>2</v>
-      </c>
-      <c r="E116" t="s" s="4">
+      <c r="D117" t="s" s="4">
+        <v>2</v>
+      </c>
+      <c r="E117" t="s" s="4">
         <v>15</v>
       </c>
-      <c r="F116" t="s" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="s" s="9">
+      <c r="F117" t="s" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s" s="9">
         <v>16</v>
       </c>
-      <c r="B117" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="C117" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="D117" t="s" s="9">
-        <v>2</v>
-      </c>
-      <c r="E117" t="s" s="9">
+      <c r="B118" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="C118" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="D118" t="s" s="9">
+        <v>2</v>
+      </c>
+      <c r="E118" t="s" s="9">
         <v>17</v>
       </c>
-      <c r="F117" t="s" s="9">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="s" s="8">
+      <c r="F118" t="s" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s" s="8">
         <v>18</v>
       </c>
-      <c r="B118" t="s" s="8">
+      <c r="B119" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="C118" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="D118" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="E118" t="s" s="8">
-        <v>2</v>
-      </c>
-      <c r="F118" t="s" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="s" s="5">
+      <c r="C119" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="D119" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="E119" t="s" s="8">
+        <v>2</v>
+      </c>
+      <c r="F119" t="s" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="B119" t="s" s="5">
+      <c r="B120" t="s" s="5">
         <v>21</v>
       </c>
-      <c r="C119" t="s" s="5">
+      <c r="C120" t="s" s="5">
         <v>22</v>
       </c>
-      <c r="D119" t="s" s="5">
+      <c r="D120" t="s" s="5">
         <v>23</v>
       </c>
-      <c r="E119" t="s" s="5">
+      <c r="E120" t="s" s="5">
         <v>24</v>
       </c>
-      <c r="F119" t="s" s="5">
+      <c r="F120" t="s" s="5">
         <v>25</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" t="n" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="B120" t="s" s="7">
-        <v>26</v>
-      </c>
-      <c r="C120" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D120" t="s" s="7">
-        <v>27</v>
-      </c>
-      <c r="E120" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F120" t="s" s="6">
-        <v>2</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="B121" t="s" s="7">
+        <v>26</v>
+      </c>
+      <c r="C121" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D121" t="s" s="7">
+        <v>27</v>
+      </c>
+      <c r="E121" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F121" t="s" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n" s="10">
         <v>2.0</v>
       </c>
-      <c r="B121" t="s" s="7">
+      <c r="B122" t="s" s="7">
         <v>28</v>
       </c>
-      <c r="C121" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="D121" t="s" s="7">
+      <c r="C122" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="D122" t="s" s="7">
         <v>78</v>
       </c>
-      <c r="E121" t="s" s="6">
-        <v>2</v>
-      </c>
-      <c r="F121" t="s" s="6">
+      <c r="E122" t="s" s="6">
+        <v>2</v>
+      </c>
+      <c r="F122" t="s" s="6">
         <v>2</v>
       </c>
     </row>
@@ -2622,14 +2642,14 @@
     <mergeCell ref="B29:F29"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B64:F64"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="B82:F82"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B65:F65"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B83:F83"/>
     <mergeCell ref="B99:D99"/>
     <mergeCell ref="B100:F100"/>
-    <mergeCell ref="B117:D117"/>
-    <mergeCell ref="B118:F118"/>
+    <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B119:F119"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>